<commit_message>
feat(hotkey): cmd shift q for cancel current process
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francorodrigo/Dropbox2nd/Ingenarte_AutoClicker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C6CD7A-E485-9842-B46C-A6451CAE4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF7CBBD-F17E-8B48-9882-DFC06E03EF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="680" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33140" yWindow="1000" windowWidth="21600" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>www.yahoo.com.ar</t>
+  </si>
+  <si>
+    <t>https://ingenarte.github.io/react-tetris2/</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -398,6 +401,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{3F9F4C5D-BAA5-0443-BCAE-020608B43355}"/>

</xml_diff>

<commit_message>
fix(debug): excesive comments from pillow reduced with warning in runmodule
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="40">
+  <fonts count="33">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -85,12 +85,6 @@
       <vertAlign val="subscript"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FFC4C4C4"/>
-      <sz val="15"/>
-    </font>
-    <font>
       <name val="Material Symbols Outlined"/>
       <color rgb="FFC4C4C4"/>
       <sz val="24"/>
@@ -114,13 +108,6 @@
       <color rgb="FFC4C4C4"/>
       <sz val="28"/>
       <vertAlign val="subscript"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF3D3D3D"/>
-      <sz val="40"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -151,21 +138,8 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF898989"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <color rgb="FF3D3D3D"/>
       <sz val="15"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF898989"/>
-      <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -212,22 +186,9 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="20"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <b val="1"/>
       <color rgb="FF000000"/>
       <sz val="20"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF74C079"/>
-      <sz val="18"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -241,12 +202,6 @@
       <family val="2"/>
       <color rgb="FF898989"/>
       <sz val="18"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF444444"/>
-      <sz val="15"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -300,38 +255,40 @@
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +470,7 @@
     <pic>
       <nvPicPr>
         <cNvPr id="1150" name="Picture 1149" descr="Aqua Turchina - _am_3450_441_1085_33840">
-          <a:hlinkClick r:id="rId3"/>
+          <a:hlinkClick r:id=""/>
         </cNvPr>
         <cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -558,7 +515,7 @@
     <pic>
       <nvPicPr>
         <cNvPr id="1151" name="Picture 1150" descr="video">
-          <a:hlinkClick r:id="rId5"/>
+          <a:hlinkClick r:id=""/>
         </cNvPr>
         <cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -603,7 +560,7 @@
     <pic>
       <nvPicPr>
         <cNvPr id="1152" name="Picture 1151" descr="Aqua Turchina - _am_3229_624_1085_33833">
-          <a:hlinkClick r:id="rId7"/>
+          <a:hlinkClick r:id=""/>
         </cNvPr>
         <cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -648,7 +605,7 @@
     <pic>
       <nvPicPr>
         <cNvPr id="1153" name="Picture 1152" descr="Aqua Turchina - _am_3271_647_1085_33842">
-          <a:hlinkClick r:id="rId9"/>
+          <a:hlinkClick r:id=""/>
         </cNvPr>
         <cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -693,7 +650,7 @@
     <pic>
       <nvPicPr>
         <cNvPr id="1154" name="Picture 1153" descr="Aqua Turchina - _am_3097_306_1085_33824">
-          <a:hlinkClick r:id="rId11"/>
+          <a:hlinkClick r:id=""/>
         </cNvPr>
         <cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -738,7 +695,7 @@
     <pic>
       <nvPicPr>
         <cNvPr id="1155" name="Picture 1154" descr="Aqua Turchina - _am_3679_hdr_559_1085_33858">
-          <a:hlinkClick r:id="rId13"/>
+          <a:hlinkClick r:id=""/>
         </cNvPr>
         <cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -5943,7 +5900,7 @@
     <pic>
       <nvPicPr>
         <cNvPr id="1364" name="Picture 1363" descr="WishSicily">
-          <a:hlinkClick tooltip="Wishsicily home" r:id="rId65"/>
+          <a:hlinkClick tooltip="Wishsicily home" r:id=""/>
         </cNvPr>
         <cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -6276,10 +6233,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2015"/>
+  <dimension ref="A1:B2015"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6320,244 +6277,7 @@
       </c>
     </row>
     <row r="10" ht="26" customHeight="1">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Villas
-Destinations
-experiences
-Guide
-search
-€EUR
-IT
-night_shelter Become host
-favorite Wishlist
-person
-Login
-Overview
-Services
-Experiences
-Area
-Press
-Reviews
-favorite
-Add to wishlist
-Enquire now
-Home All our villas in Sicily Aqua Turchina
-Aqua Turchina
-5 reviews
-share
-Share
-favorite
-Add to wishlist
-location_on Cefalù (Palermo)CIN: IT082059B42RRFDL3J
-1 of 51
-hotel
-4
-group
-8
-bathtub
-3
-straighten
-150 sq m
-“
-Contemporary style, recently renovated, and direct beach access.
-Aqua Turchina is a seafront villa with direct beach access, pool, table tennis, and ample outdoor space. It features four bedrooms, three bathrooms, and is near Finale di Pollina and Cefalù.
-read more
-Overview
-With direct access through a garden gate on to a pebbly beach, Aqua Turchina is a delightful seafront villa with a pool, table tennis and plenty of outdoor space. The four-bedroom, three-bathroom villa also has the advantage of being close to the pizzerias, restaurants and shops at Finale di Pollina and is ideally situated for day trips to the vibrant seaside resort of Cefalù (20km), to Palermo and the Madonie Mountains.
-Suitable for either families or groups of friends, there’s ample garden space to relax back on comfy sun beds while the more energetic members of the group splash in the pool or play table tennis. In addition to the sun beds on the lawn, there’s a charming decked hideaway, set amongst mature trees and foliage, and close to the gate to the beach, which is the perfect retreat for an afternoon snooze! Top and tail your day with leisurely breakfasts on the lounge seating on the spacious veranda and al fresco dinners, set against a backdrop of the sound of the ocean. In addition to the lounge seating and a dining table and chairs, the veranda has a well-equipped outdoor kitchen, complete with barbecue, sink and storage space.
-Step into a contemporary villa furnished throughout with porcelain tiled floors and a pleasing restful palette of gentle shades of grey. The main open plan living space is filled with natural light thanks to its large sea-facing windows and features a sofa and an open plan kitchen with a worktop that doubles up as a breakfast bar.
-All the bedrooms are attractively furnished, and bathrooms feature stylish tiling and contemporary bathroom fittings, including showers. The sleeping area comprises three generously sized double bedrooms (two en-suite) and one twin bedroom (can be converted to a double). A third bathroom is available for the third and fourth bedroom.
- Day area
-Blender
-Bookshelves
-Coffee machine
-Crockery
-Detergents and cleaners
-Dishwasher
-Freezer
-Iron and ironing board
-Kettle
-Microwave
-Moka
-Oven
-Refrigerator
-SMART TV
-Toaster
-Washing machine
-show all
- Night area
-Baby bed
-Bath Towels
-Detergents and toilet paper
-Double bedrooms
-En-suite bathroom
-Hairdryer
-Linen
-Twin bedrooms
- Outdoors
-Barbecue
-Deckchairs
-Garden
-Outdoor kitchen
-Outdoor shower
-Private parking
-Private swimming pool
-Terrace
- Other amenities
-Air conditioning
-Beach umbrella and chairs
-Board games
-Canoe
-Central heating
-Electric vehicle charger
-Highchair
-Insect repellents
-Internet Wi-Fi
-Non-smoking
-Pay per view (Sky, Netflix or Premium)
-Ping pong table
-Pool towels
-Rowing Boat
-Weekly cleaning
-Welcome hamper
-show all
-Good to know
-info
-How to pay for your stay
-property listing
-check
-Additional notes
-and house rules
-room_service
-Extra costs
-and what to pay upon arrival
-bolt
-Sicily Experiences Trio
-Save on a package of 3 Active Experiences
-Area
-This unique beachfront villa is located a short drive from Finale di Pollina (2km), a charming seaside village on the north coast of Sicily, where you can get everything you need from a good selection of shops, restaurants, trattorie, pizzerie and bars. The beach is literally on your doorstep and the panoramic terrace enjoys a splendid view of the whole coast.
-A quick 15-minute motorway drive takes you to the seaside resort of Cefalù. This is one of Sicily’s busier towns, particularly during the summer months, thanks to its fish restaurants, shops and fabulous beaches. However, a visit here is enjoyable at any time of year thanks to its UNESCO world heritage Norman cathedral and its medieval town centre. Banks, shops and supermarkets are all available here. Continuing west along the coast, you reach Palermo (just over an hour) where there are some superb sightseeing opportunities and, of course, the city’s famous street food markets.
-If you like the idea of leaving the car behind and hopping on a train, the recently opened Finale di Pollina railway station is just 5 minutes’ walk away. The small electric train connects a series of towns along Sicily’s north coast, from Palermo to Messina and including Cefalu. Despite the proximity to the station, the train can barely be heard.
-A little further afield, though little more than an hour away, the Greek temple and theatre at Segesta is well worth a visit. Other local archaeological sites include Himera which is less than 40 minutes by car. If you feel like getting right off the beaten track, the Madonie National Park is a glorious spot for hiking, great views or exploring medieval hilltop towns such as Polizzi Generosa or Petralia Soprana.
-A brand-new spot has just opened in Costa Turchina: Beach Club Costa Turchina, a laid-back restaurant and lounge bar. It's just a short walk from the villa, making it easy to enjoy a pizza, a seafood dinner, or a relaxed drink in the evening. Additionally, the Beach Club offers rentals of electric bikes, scooters, and boats, so you can explore the area with complete freedom. A great addition to make your stay even more enjoyable!
-read more
-favorite
-Add to wishlist
-5 (5 Reviews)
-Check-in
-pick a date
-Check-out
-pick a date
-Guests
-0 adult 0 child 0 infant 0 pet
-Bedrooms
-0 bedroom
-Price per night from
-€ 260.00
-Book online
-Enquire now
-Discover
-Discover places of interest and services near Aqua Turchina
-Food
-Health
-Amenities
-Tourist attractions
-Reset
-add
-remove
-Surroundings
-Cefalù
-Experiences
-Book one of our Experiences with Aqua Turchina
-discover all experiences
-Press
-Aqua Turchina appeared on these articles
-Wish Sicily in the Daily Mail with Villa Aqua Turchina
-The hottest last-minute summer holidays under £1000pp Wish Sicily’s Aqua Turchina was in prime posi...
-Reviews
-5/5 100% genuine
-Leave a review
-Trusted c.
-November 2024
-Excellent accommodation
-Everything good. Excellent accommodation :) Very friendly
-Roberto M.
-September 2024
-Il nostro soggiorno ad Aqua Turchina è stato davvero piacevole. L'agenzia si è dimostrata efficiente e disponibile, rispondendo prontamente a ogni richiesta. La villa è in una posizione fantastica, con accesso diretto al mare, e una terrazza che offre una bella vista. Avere la spiaggia così vicina è stato un grande vantaggio, e la breve distanza da Finale di Pollina ci ha permesso di visitare facilmente il paese. Un'esperienza che consigliamo per una vacanza rilassante. Il nostro soggiorno ad Aqua Turchina è stato davvero piacevole. L'agenzia si è dimostrata efficiente e disponibile, rispondendo prontamente a ogni richiesta. La villa è in una posizione fantastica, con accesso diretto al mare, e una terrazza che offre una bella vista. Avere la spiaggia così vicina è stato un grande vantaggio, e la breve distanza da Finale di Pollina ci ha permesso di visitare facilmente il paese. Un'esperienza che consigliamo per una vacanza rilassante.
-read more
-Natalie J.
-August 2024
-Perfect vacation spot when traveling with family of all ages! Very clean house with private beach access ☀️ Friendly host who helped with local recommendations and even walked us to our first dinner reservation. Would definitely recommend their beautiful home to anyone going to the area! One suggestion - Make sure you’re familiar with European appliances before arrival!
-read more
-Trusted c.
-July 2024
-HOLIDAY WEEK IN FINALE DI POLLINA
-PERFECT ACCOMODATION IN FRONT OF STUNNING SEA BEAUTIFUL HOUSE WITH ALL NEEDED AMENITIES NICE GARDEN AND POOL SPECIAL THANKS TO MR FRANCESCO ( OWNER OF THE HOUSE ) THAT WAS ALWAYS AVAILABLE AND REACHABLE FOR ALL OUR NEED AND INFORMATION TRYING TO SATISFY ALL OUR NEEDED AND REQUEST VERY HELPFUL AND ALWAYS AVAILABLE FOR ALL OUR RQUEST AND SUPPORT NEEDED
-read more
-agostino d.
-September 2023
-Abbiamo soggiornato in questo stupendo luogo subito dopo ferragosto, per una settimana. Acqua splendida, casa ottima con tutto quello che serve, location veramente stupenda. Il proprietario, Francesco, è persona gentilissima e molto disponibile. E i dintorni, le Madonie e Cefalù, veramente da visitare. Ottima scelta
-read more
-5 of 5 reviews
-Enquire now
-Aqua Turchina
-5 Reviews
-location_on Cefalù (Palermo)
-Name 
-Surname 
-Nationality 
-Italy
-Phone 
-Italy +39
-+39
-312 345 6789
-Email 
-Check-in
-Check-out
-pick a date
-pick a date
- I don't have a date scheduled
-Guests
-0 adult 0 child 0 infant 0 pet
-Bedrooms
-0 bedroom
-Message 
- I've read and agree to the Privacy Policy and the Terms &amp; Conditions
-Send request
-Your wish for a villa escape
-About us
-Contact us
-Who we are
-What the Press says
-FAQ
-Customers
-Villas
-Experiences
-Guide to Sicily
-Car hire
-Destinations
-North: Sea and Mountains
-East: Land of Etna
-West: History and Wines
-South: Golden Coast
-South-East: Val di Noto
-Owners
-List your property
-General terms of use
-Advice to owners
-Why Wish Sicily
-Support Sicily srl
-VAT IT06182930823
-Via Uditore, 11/H, 90145
-Palermo, Italy
-© 2025 Wish Sicily · Terms &amp; conditions · Privacy policy · Press room · Collections
-€EUR
-IT
-</t>
-        </is>
-      </c>
+      <c r="A10" s="33" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
@@ -6566,16 +6286,29 @@
       <c r="A12" s="1" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n"/>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>260.00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n"/>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>260.00</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
-      <c r="A16" s="3" t="n"/>
+      <c r="A16" s="2" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
@@ -6614,396 +6347,396 @@
       <c r="A28" s="1" t="n"/>
     </row>
     <row r="29" ht="20" customHeight="1">
-      <c r="A29" s="4" t="n"/>
+      <c r="A29" s="3" t="n"/>
     </row>
     <row r="30" ht="49" customHeight="1">
-      <c r="A30" s="5" t="n"/>
+      <c r="A30" s="4" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
     </row>
     <row r="32" ht="27" customHeight="1">
-      <c r="A32" s="7" t="n"/>
+      <c r="A32" s="6" t="n"/>
     </row>
     <row r="33" ht="34" customHeight="1">
-      <c r="A33" s="8" t="n"/>
+      <c r="A33" s="7" t="n"/>
     </row>
     <row r="34" ht="20" customHeight="1">
-      <c r="A34" s="9" t="n"/>
+      <c r="A34" s="8" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="n"/>
+      <c r="A35" s="9" t="n"/>
     </row>
     <row r="36" ht="20" customHeight="1">
-      <c r="A36" s="4" t="n"/>
+      <c r="A36" s="3" t="n"/>
     </row>
     <row r="62" ht="20" customHeight="1">
-      <c r="A62" s="4" t="n"/>
+      <c r="A62" s="3" t="n"/>
     </row>
     <row r="63" ht="20" customHeight="1">
-      <c r="A63" s="4" t="n"/>
+      <c r="A63" s="3" t="n"/>
     </row>
     <row r="89" ht="20" customHeight="1">
-      <c r="A89" s="4" t="n"/>
+      <c r="A89" s="3" t="n"/>
     </row>
     <row r="90" ht="20" customHeight="1">
-      <c r="A90" s="4" t="n"/>
+      <c r="A90" s="3" t="n"/>
     </row>
     <row r="116" ht="20" customHeight="1">
-      <c r="A116" s="4" t="n"/>
+      <c r="A116" s="3" t="n"/>
     </row>
     <row r="117" ht="20" customHeight="1">
-      <c r="A117" s="4" t="n"/>
+      <c r="A117" s="3" t="n"/>
     </row>
     <row r="146" ht="20" customHeight="1">
-      <c r="A146" s="4" t="n"/>
+      <c r="A146" s="3" t="n"/>
     </row>
     <row r="147" ht="20" customHeight="1">
-      <c r="A147" s="4" t="n"/>
+      <c r="A147" s="3" t="n"/>
     </row>
     <row r="173" ht="20" customHeight="1">
-      <c r="A173" s="4" t="n"/>
+      <c r="A173" s="3" t="n"/>
     </row>
     <row r="174" ht="20" customHeight="1">
-      <c r="A174" s="4" t="n"/>
+      <c r="A174" s="3" t="n"/>
     </row>
     <row r="200" ht="20" customHeight="1">
-      <c r="A200" s="4" t="n"/>
+      <c r="A200" s="3" t="n"/>
     </row>
     <row r="201" ht="20" customHeight="1">
-      <c r="A201" s="4" t="n"/>
+      <c r="A201" s="3" t="n"/>
     </row>
     <row r="227" ht="20" customHeight="1">
-      <c r="A227" s="4" t="n"/>
+      <c r="A227" s="3" t="n"/>
     </row>
     <row r="228" ht="20" customHeight="1">
-      <c r="A228" s="4" t="n"/>
+      <c r="A228" s="3" t="n"/>
     </row>
     <row r="254" ht="20" customHeight="1">
-      <c r="A254" s="4" t="n"/>
+      <c r="A254" s="3" t="n"/>
     </row>
     <row r="255" ht="20" customHeight="1">
-      <c r="A255" s="4" t="n"/>
+      <c r="A255" s="3" t="n"/>
     </row>
     <row r="281" ht="20" customHeight="1">
-      <c r="A281" s="4" t="n"/>
+      <c r="A281" s="3" t="n"/>
     </row>
     <row r="282" ht="20" customHeight="1">
-      <c r="A282" s="4" t="n"/>
+      <c r="A282" s="3" t="n"/>
     </row>
     <row r="308" ht="20" customHeight="1">
-      <c r="A308" s="4" t="n"/>
+      <c r="A308" s="3" t="n"/>
     </row>
     <row r="309" ht="20" customHeight="1">
-      <c r="A309" s="4" t="n"/>
+      <c r="A309" s="3" t="n"/>
     </row>
     <row r="335" ht="20" customHeight="1">
-      <c r="A335" s="4" t="n"/>
+      <c r="A335" s="3" t="n"/>
     </row>
     <row r="336" ht="20" customHeight="1">
-      <c r="A336" s="4" t="n"/>
+      <c r="A336" s="3" t="n"/>
     </row>
     <row r="362" ht="20" customHeight="1">
-      <c r="A362" s="4" t="n"/>
+      <c r="A362" s="3" t="n"/>
     </row>
     <row r="363" ht="20" customHeight="1">
-      <c r="A363" s="4" t="n"/>
+      <c r="A363" s="3" t="n"/>
     </row>
     <row r="389" ht="20" customHeight="1">
-      <c r="A389" s="4" t="n"/>
+      <c r="A389" s="3" t="n"/>
     </row>
     <row r="390" ht="20" customHeight="1">
-      <c r="A390" s="4" t="n"/>
+      <c r="A390" s="3" t="n"/>
     </row>
     <row r="416" ht="20" customHeight="1">
-      <c r="A416" s="4" t="n"/>
+      <c r="A416" s="3" t="n"/>
     </row>
     <row r="417" ht="20" customHeight="1">
-      <c r="A417" s="4" t="n"/>
+      <c r="A417" s="3" t="n"/>
     </row>
     <row r="443" ht="20" customHeight="1">
-      <c r="A443" s="4" t="n"/>
+      <c r="A443" s="3" t="n"/>
     </row>
     <row r="444" ht="20" customHeight="1">
-      <c r="A444" s="4" t="n"/>
+      <c r="A444" s="3" t="n"/>
     </row>
     <row r="470" ht="20" customHeight="1">
-      <c r="A470" s="4" t="n"/>
+      <c r="A470" s="3" t="n"/>
     </row>
     <row r="471" ht="20" customHeight="1">
-      <c r="A471" s="4" t="n"/>
+      <c r="A471" s="3" t="n"/>
     </row>
     <row r="497" ht="20" customHeight="1">
-      <c r="A497" s="4" t="n"/>
+      <c r="A497" s="3" t="n"/>
     </row>
     <row r="498" ht="20" customHeight="1">
-      <c r="A498" s="4" t="n"/>
+      <c r="A498" s="3" t="n"/>
     </row>
     <row r="524" ht="20" customHeight="1">
-      <c r="A524" s="4" t="n"/>
+      <c r="A524" s="3" t="n"/>
     </row>
     <row r="525" ht="20" customHeight="1">
-      <c r="A525" s="4" t="n"/>
+      <c r="A525" s="3" t="n"/>
     </row>
     <row r="551" ht="20" customHeight="1">
-      <c r="A551" s="4" t="n"/>
+      <c r="A551" s="3" t="n"/>
     </row>
     <row r="552" ht="20" customHeight="1">
-      <c r="A552" s="4" t="n"/>
+      <c r="A552" s="3" t="n"/>
     </row>
     <row r="578" ht="20" customHeight="1">
-      <c r="A578" s="4" t="n"/>
+      <c r="A578" s="3" t="n"/>
     </row>
     <row r="579" ht="20" customHeight="1">
-      <c r="A579" s="4" t="n"/>
+      <c r="A579" s="3" t="n"/>
     </row>
     <row r="605" ht="20" customHeight="1">
-      <c r="A605" s="4" t="n"/>
+      <c r="A605" s="3" t="n"/>
     </row>
     <row r="606" ht="20" customHeight="1">
-      <c r="A606" s="4" t="n"/>
+      <c r="A606" s="3" t="n"/>
     </row>
     <row r="632" ht="20" customHeight="1">
-      <c r="A632" s="4" t="n"/>
+      <c r="A632" s="3" t="n"/>
     </row>
     <row r="633" ht="20" customHeight="1">
-      <c r="A633" s="4" t="n"/>
+      <c r="A633" s="3" t="n"/>
     </row>
     <row r="659" ht="20" customHeight="1">
-      <c r="A659" s="4" t="n"/>
+      <c r="A659" s="3" t="n"/>
     </row>
     <row r="660" ht="20" customHeight="1">
-      <c r="A660" s="4" t="n"/>
+      <c r="A660" s="3" t="n"/>
     </row>
     <row r="686" ht="20" customHeight="1">
-      <c r="A686" s="4" t="n"/>
+      <c r="A686" s="3" t="n"/>
     </row>
     <row r="687" ht="20" customHeight="1">
-      <c r="A687" s="4" t="n"/>
+      <c r="A687" s="3" t="n"/>
     </row>
     <row r="713" ht="20" customHeight="1">
-      <c r="A713" s="4" t="n"/>
+      <c r="A713" s="3" t="n"/>
     </row>
     <row r="714" ht="20" customHeight="1">
-      <c r="A714" s="4" t="n"/>
+      <c r="A714" s="3" t="n"/>
     </row>
     <row r="740" ht="20" customHeight="1">
-      <c r="A740" s="4" t="n"/>
+      <c r="A740" s="3" t="n"/>
     </row>
     <row r="741" ht="20" customHeight="1">
-      <c r="A741" s="4" t="n"/>
+      <c r="A741" s="3" t="n"/>
     </row>
     <row r="767" ht="20" customHeight="1">
-      <c r="A767" s="4" t="n"/>
+      <c r="A767" s="3" t="n"/>
     </row>
     <row r="768" ht="20" customHeight="1">
-      <c r="A768" s="4" t="n"/>
+      <c r="A768" s="3" t="n"/>
     </row>
     <row r="794" ht="20" customHeight="1">
-      <c r="A794" s="4" t="n"/>
+      <c r="A794" s="3" t="n"/>
     </row>
     <row r="795" ht="20" customHeight="1">
-      <c r="A795" s="4" t="n"/>
+      <c r="A795" s="3" t="n"/>
     </row>
     <row r="821" ht="20" customHeight="1">
-      <c r="A821" s="4" t="n"/>
+      <c r="A821" s="3" t="n"/>
     </row>
     <row r="822" ht="20" customHeight="1">
-      <c r="A822" s="4" t="n"/>
+      <c r="A822" s="3" t="n"/>
     </row>
     <row r="848" ht="20" customHeight="1">
-      <c r="A848" s="4" t="n"/>
+      <c r="A848" s="3" t="n"/>
     </row>
     <row r="849" ht="20" customHeight="1">
-      <c r="A849" s="4" t="n"/>
+      <c r="A849" s="3" t="n"/>
     </row>
     <row r="875" ht="20" customHeight="1">
-      <c r="A875" s="4" t="n"/>
+      <c r="A875" s="3" t="n"/>
     </row>
     <row r="876" ht="20" customHeight="1">
-      <c r="A876" s="4" t="n"/>
+      <c r="A876" s="3" t="n"/>
     </row>
     <row r="902" ht="20" customHeight="1">
-      <c r="A902" s="4" t="n"/>
+      <c r="A902" s="3" t="n"/>
     </row>
     <row r="903" ht="20" customHeight="1">
-      <c r="A903" s="4" t="n"/>
+      <c r="A903" s="3" t="n"/>
     </row>
     <row r="929" ht="20" customHeight="1">
-      <c r="A929" s="4" t="n"/>
+      <c r="A929" s="3" t="n"/>
     </row>
     <row r="930" ht="20" customHeight="1">
-      <c r="A930" s="4" t="n"/>
+      <c r="A930" s="3" t="n"/>
     </row>
     <row r="956" ht="20" customHeight="1">
-      <c r="A956" s="4" t="n"/>
+      <c r="A956" s="3" t="n"/>
     </row>
     <row r="957" ht="20" customHeight="1">
-      <c r="A957" s="4" t="n"/>
+      <c r="A957" s="3" t="n"/>
     </row>
     <row r="983" ht="20" customHeight="1">
-      <c r="A983" s="4" t="n"/>
+      <c r="A983" s="3" t="n"/>
     </row>
     <row r="984" ht="20" customHeight="1">
-      <c r="A984" s="4" t="n"/>
+      <c r="A984" s="3" t="n"/>
     </row>
     <row r="1010" ht="20" customHeight="1">
-      <c r="A1010" s="4" t="n"/>
+      <c r="A1010" s="3" t="n"/>
     </row>
     <row r="1011" ht="20" customHeight="1">
-      <c r="A1011" s="4" t="n"/>
+      <c r="A1011" s="3" t="n"/>
     </row>
     <row r="1037" ht="20" customHeight="1">
-      <c r="A1037" s="4" t="n"/>
+      <c r="A1037" s="3" t="n"/>
     </row>
     <row r="1038" ht="20" customHeight="1">
-      <c r="A1038" s="4" t="n"/>
+      <c r="A1038" s="3" t="n"/>
     </row>
     <row r="1064" ht="20" customHeight="1">
-      <c r="A1064" s="4" t="n"/>
+      <c r="A1064" s="3" t="n"/>
     </row>
     <row r="1065" ht="20" customHeight="1">
-      <c r="A1065" s="4" t="n"/>
+      <c r="A1065" s="3" t="n"/>
     </row>
     <row r="1091" ht="20" customHeight="1">
-      <c r="A1091" s="4" t="n"/>
+      <c r="A1091" s="3" t="n"/>
     </row>
     <row r="1092" ht="20" customHeight="1">
-      <c r="A1092" s="4" t="n"/>
+      <c r="A1092" s="3" t="n"/>
     </row>
     <row r="1118" ht="20" customHeight="1">
-      <c r="A1118" s="4" t="n"/>
+      <c r="A1118" s="3" t="n"/>
     </row>
     <row r="1119" ht="20" customHeight="1">
-      <c r="A1119" s="4" t="n"/>
+      <c r="A1119" s="3" t="n"/>
     </row>
     <row r="1145" ht="20" customHeight="1">
-      <c r="A1145" s="4" t="n"/>
+      <c r="A1145" s="3" t="n"/>
     </row>
     <row r="1146" ht="20" customHeight="1">
-      <c r="A1146" s="4" t="n"/>
+      <c r="A1146" s="3" t="n"/>
     </row>
     <row r="1172" ht="20" customHeight="1">
-      <c r="A1172" s="4" t="n"/>
+      <c r="A1172" s="3" t="n"/>
     </row>
     <row r="1173" ht="20" customHeight="1">
-      <c r="A1173" s="4" t="n"/>
+      <c r="A1173" s="3" t="n"/>
     </row>
     <row r="1199" ht="20" customHeight="1">
-      <c r="A1199" s="4" t="n"/>
+      <c r="A1199" s="3" t="n"/>
     </row>
     <row r="1200" ht="20" customHeight="1">
-      <c r="A1200" s="4" t="n"/>
+      <c r="A1200" s="3" t="n"/>
     </row>
     <row r="1226" ht="20" customHeight="1">
-      <c r="A1226" s="4" t="n"/>
+      <c r="A1226" s="3" t="n"/>
     </row>
     <row r="1227" ht="20" customHeight="1">
-      <c r="A1227" s="4" t="n"/>
+      <c r="A1227" s="3" t="n"/>
     </row>
     <row r="1253" ht="20" customHeight="1">
-      <c r="A1253" s="4" t="n"/>
+      <c r="A1253" s="3" t="n"/>
     </row>
     <row r="1254" ht="20" customHeight="1">
-      <c r="A1254" s="4" t="n"/>
+      <c r="A1254" s="3" t="n"/>
     </row>
     <row r="1280" ht="20" customHeight="1">
-      <c r="A1280" s="4" t="n"/>
+      <c r="A1280" s="3" t="n"/>
     </row>
     <row r="1281" ht="20" customHeight="1">
-      <c r="A1281" s="4" t="n"/>
+      <c r="A1281" s="3" t="n"/>
     </row>
     <row r="1307" ht="20" customHeight="1">
-      <c r="A1307" s="4" t="n"/>
+      <c r="A1307" s="3" t="n"/>
     </row>
     <row r="1308" ht="20" customHeight="1">
-      <c r="A1308" s="4" t="n"/>
+      <c r="A1308" s="3" t="n"/>
     </row>
     <row r="1334" ht="20" customHeight="1">
-      <c r="A1334" s="4" t="n"/>
+      <c r="A1334" s="3" t="n"/>
     </row>
     <row r="1335" ht="20" customHeight="1">
-      <c r="A1335" s="4" t="n"/>
+      <c r="A1335" s="3" t="n"/>
     </row>
     <row r="1361" ht="20" customHeight="1">
-      <c r="A1361" s="4" t="n"/>
+      <c r="A1361" s="3" t="n"/>
     </row>
     <row r="1362" ht="20" customHeight="1">
-      <c r="A1362" s="4" t="n"/>
+      <c r="A1362" s="3" t="n"/>
     </row>
     <row r="1388" ht="20" customHeight="1">
-      <c r="A1388" s="4" t="n"/>
+      <c r="A1388" s="3" t="n"/>
     </row>
     <row r="1389" ht="20" customHeight="1">
-      <c r="A1389" s="4" t="n"/>
+      <c r="A1389" s="3" t="n"/>
     </row>
     <row r="1415" ht="20" customHeight="1">
-      <c r="A1415" s="4" t="n"/>
+      <c r="A1415" s="3" t="n"/>
     </row>
     <row r="1416" ht="20" customHeight="1">
-      <c r="A1416" s="4" t="n"/>
+      <c r="A1416" s="3" t="n"/>
     </row>
     <row r="1442" ht="20" customHeight="1">
-      <c r="A1442" s="4" t="n"/>
+      <c r="A1442" s="3" t="n"/>
     </row>
     <row r="1443" ht="20" customHeight="1">
-      <c r="A1443" s="4" t="n"/>
+      <c r="A1443" s="3" t="n"/>
     </row>
     <row r="1469" ht="20" customHeight="1">
-      <c r="A1469" s="4" t="n"/>
+      <c r="A1469" s="3" t="n"/>
     </row>
     <row r="1470" ht="20" customHeight="1">
-      <c r="A1470" s="4" t="n"/>
+      <c r="A1470" s="3" t="n"/>
     </row>
     <row r="1496" ht="20" customHeight="1">
-      <c r="A1496" s="4" t="n"/>
+      <c r="A1496" s="3" t="n"/>
     </row>
     <row r="1497" ht="20" customHeight="1">
-      <c r="A1497" s="4" t="n"/>
+      <c r="A1497" s="3" t="n"/>
     </row>
     <row r="1526" ht="20" customHeight="1">
-      <c r="A1526" s="4" t="n"/>
+      <c r="A1526" s="3" t="n"/>
     </row>
     <row r="1527" ht="20" customHeight="1">
-      <c r="A1527" s="4" t="n"/>
+      <c r="A1527" s="3" t="n"/>
     </row>
     <row r="1553" ht="20" customHeight="1">
-      <c r="A1553" s="4" t="n"/>
+      <c r="A1553" s="3" t="n"/>
     </row>
     <row r="1554" ht="20" customHeight="1">
-      <c r="A1554" s="4" t="n"/>
+      <c r="A1554" s="3" t="n"/>
     </row>
     <row r="1580" ht="20" customHeight="1">
-      <c r="A1580" s="11" t="n"/>
+      <c r="A1580" s="10" t="n"/>
     </row>
     <row r="1581" ht="20" customHeight="1">
-      <c r="A1581" s="11" t="n"/>
+      <c r="A1581" s="10" t="n"/>
     </row>
     <row r="1610" ht="20" customHeight="1">
-      <c r="A1610" s="11" t="n"/>
+      <c r="A1610" s="10" t="n"/>
     </row>
     <row r="1611" ht="20" customHeight="1">
-      <c r="A1611" s="11" t="n"/>
+      <c r="A1611" s="10" t="n"/>
     </row>
     <row r="1612" ht="20" customHeight="1">
-      <c r="A1612" s="11" t="n"/>
+      <c r="A1612" s="10" t="n"/>
     </row>
     <row r="1642" ht="41" customHeight="1">
-      <c r="A1642" s="12" t="inlineStr">
+      <c r="A1642" s="11" t="inlineStr">
         <is>
           <t>hotel4group8bathtub3straighten150 sq m</t>
         </is>
       </c>
     </row>
     <row r="1645" ht="74" customHeight="1">
-      <c r="A1645" s="13" t="inlineStr">
+      <c r="A1645" s="12" t="inlineStr">
         <is>
           <t>“Contemporary style, recently renovated, and direct beach access.</t>
         </is>
       </c>
     </row>
     <row r="1648" ht="20" customHeight="1">
-      <c r="A1648" s="4" t="inlineStr">
+      <c r="A1648" s="3" t="inlineStr">
         <is>
           <t>Aqua Turchina is a seafront villa with direct beach access, pool, table tennis, and ample outdoor space. It features four bedrooms, three bathrooms, and is near Finale di Pollina and Cefalù.</t>
         </is>
@@ -7017,160 +6750,160 @@
       </c>
     </row>
     <row r="1651" ht="20" customHeight="1">
-      <c r="A1651" s="4" t="n"/>
+      <c r="A1651" s="3" t="n"/>
     </row>
     <row r="1652" ht="20" customHeight="1">
-      <c r="A1652" s="4" t="n"/>
+      <c r="A1652" s="3" t="n"/>
     </row>
     <row r="1661" ht="31" customHeight="1">
-      <c r="A1661" s="14" t="inlineStr">
+      <c r="A1661" s="13" t="inlineStr">
         <is>
           <t>Overview</t>
         </is>
       </c>
     </row>
     <row r="1663" ht="20" customHeight="1">
-      <c r="A1663" s="4" t="inlineStr">
+      <c r="A1663" s="3" t="inlineStr">
         <is>
           <t>With direct access through a garden gate on to a pebbly beach, Aqua Turchina is a delightful seafront villa with a pool, table tennis and plenty of outdoor space. The four-bedroom, three-bathroom villa also has the advantage of being close to the pizzerias, restaurants and shops at Finale di Pollina and is ideally situated for day trips to the vibrant seaside resort of Cefalù (20km), to Palermo and the Madonie Mountains.</t>
         </is>
       </c>
     </row>
     <row r="1665" ht="20" customHeight="1">
-      <c r="A1665" s="4" t="inlineStr">
+      <c r="A1665" s="3" t="inlineStr">
         <is>
           <t>Suitable for either families or groups of friends, there’s ample garden space to relax back on comfy sun beds while the more energetic members of the group splash in the pool or play table tennis. In addition to the sun beds on the lawn, there’s a charming decked hideaway, set amongst mature trees and foliage, and close to the gate to the beach, which is the perfect retreat for an afternoon snooze! Top and tail your day with leisurely breakfasts on the lounge seating on the spacious veranda and al fresco dinners, set against a backdrop of the sound of the ocean. In addition to the lounge seating and a dining table and chairs, the veranda has a well-equipped outdoor kitchen, complete with barbecue, sink and storage space.</t>
         </is>
       </c>
     </row>
     <row r="1667" ht="20" customHeight="1">
-      <c r="A1667" s="4" t="inlineStr">
+      <c r="A1667" s="3" t="inlineStr">
         <is>
           <t>Step into a contemporary villa furnished throughout with porcelain tiled floors and a pleasing restful palette of gentle shades of grey. The main open plan living space is filled with natural light thanks to its large sea-facing windows and features a sofa and an open plan kitchen with a worktop that doubles up as a breakfast bar.</t>
         </is>
       </c>
     </row>
     <row r="1669" ht="20" customHeight="1">
-      <c r="A1669" s="4" t="inlineStr">
+      <c r="A1669" s="3" t="inlineStr">
         <is>
           <t>All the bedrooms are attractively furnished, and bathrooms feature stylish tiling and contemporary bathroom fittings, including showers. The sleeping area comprises three generously sized double bedrooms (two en-suite) and one twin bedroom (can be converted to a double). A third bathroom is available for the third and fourth bedroom.</t>
         </is>
       </c>
     </row>
     <row r="1671" ht="31" customHeight="1">
-      <c r="A1671" s="14" t="inlineStr">
+      <c r="A1671" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve"> Day area</t>
         </is>
       </c>
     </row>
     <row r="1672" ht="20" customHeight="1">
-      <c r="A1672" s="4" t="inlineStr">
+      <c r="A1672" s="3" t="inlineStr">
         <is>
           <t>Blender</t>
         </is>
       </c>
     </row>
     <row r="1673" ht="20" customHeight="1">
-      <c r="A1673" s="4" t="inlineStr">
+      <c r="A1673" s="3" t="inlineStr">
         <is>
           <t>Bookshelves</t>
         </is>
       </c>
     </row>
     <row r="1674" ht="20" customHeight="1">
-      <c r="A1674" s="4" t="inlineStr">
+      <c r="A1674" s="3" t="inlineStr">
         <is>
           <t>Coffee machine</t>
         </is>
       </c>
     </row>
     <row r="1675" ht="20" customHeight="1">
-      <c r="A1675" s="4" t="inlineStr">
+      <c r="A1675" s="3" t="inlineStr">
         <is>
           <t>Crockery</t>
         </is>
       </c>
     </row>
     <row r="1676" ht="20" customHeight="1">
-      <c r="A1676" s="4" t="inlineStr">
+      <c r="A1676" s="3" t="inlineStr">
         <is>
           <t>Detergents and cleaners</t>
         </is>
       </c>
     </row>
     <row r="1677" ht="20" customHeight="1">
-      <c r="A1677" s="4" t="inlineStr">
+      <c r="A1677" s="3" t="inlineStr">
         <is>
           <t>Dishwasher</t>
         </is>
       </c>
     </row>
     <row r="1678" ht="20" customHeight="1">
-      <c r="A1678" s="4" t="inlineStr">
+      <c r="A1678" s="3" t="inlineStr">
         <is>
           <t>Freezer</t>
         </is>
       </c>
     </row>
     <row r="1679" ht="20" customHeight="1">
-      <c r="A1679" s="4" t="inlineStr">
+      <c r="A1679" s="3" t="inlineStr">
         <is>
           <t>Iron and ironing board</t>
         </is>
       </c>
     </row>
     <row r="1680" ht="20" customHeight="1">
-      <c r="A1680" s="4" t="inlineStr">
+      <c r="A1680" s="3" t="inlineStr">
         <is>
           <t>Kettle</t>
         </is>
       </c>
     </row>
     <row r="1681" ht="20" customHeight="1">
-      <c r="A1681" s="4" t="inlineStr">
+      <c r="A1681" s="3" t="inlineStr">
         <is>
           <t>Microwave</t>
         </is>
       </c>
     </row>
     <row r="1682" ht="20" customHeight="1">
-      <c r="A1682" s="4" t="inlineStr">
+      <c r="A1682" s="3" t="inlineStr">
         <is>
           <t>Moka</t>
         </is>
       </c>
     </row>
     <row r="1683" ht="20" customHeight="1">
-      <c r="A1683" s="4" t="inlineStr">
+      <c r="A1683" s="3" t="inlineStr">
         <is>
           <t>Oven</t>
         </is>
       </c>
     </row>
     <row r="1684" ht="20" customHeight="1">
-      <c r="A1684" s="4" t="inlineStr">
+      <c r="A1684" s="3" t="inlineStr">
         <is>
           <t>Refrigerator</t>
         </is>
       </c>
     </row>
     <row r="1685" ht="20" customHeight="1">
-      <c r="A1685" s="4" t="inlineStr">
+      <c r="A1685" s="3" t="inlineStr">
         <is>
           <t>SMART TV</t>
         </is>
       </c>
     </row>
     <row r="1686" ht="20" customHeight="1">
-      <c r="A1686" s="4" t="inlineStr">
+      <c r="A1686" s="3" t="inlineStr">
         <is>
           <t>Toaster</t>
         </is>
       </c>
     </row>
     <row r="1687" ht="20" customHeight="1">
-      <c r="A1687" s="4" t="inlineStr">
+      <c r="A1687" s="3" t="inlineStr">
         <is>
           <t>Washing machine</t>
         </is>
@@ -7184,245 +6917,245 @@
       </c>
     </row>
     <row r="1689" ht="31" customHeight="1">
-      <c r="A1689" s="14" t="inlineStr">
+      <c r="A1689" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve"> Night area</t>
         </is>
       </c>
     </row>
     <row r="1690" ht="20" customHeight="1">
-      <c r="A1690" s="4" t="inlineStr">
+      <c r="A1690" s="3" t="inlineStr">
         <is>
           <t>Baby bed</t>
         </is>
       </c>
     </row>
     <row r="1691" ht="20" customHeight="1">
-      <c r="A1691" s="4" t="inlineStr">
+      <c r="A1691" s="3" t="inlineStr">
         <is>
           <t>Bath Towels</t>
         </is>
       </c>
     </row>
     <row r="1692" ht="20" customHeight="1">
-      <c r="A1692" s="4" t="inlineStr">
+      <c r="A1692" s="3" t="inlineStr">
         <is>
           <t>Detergents and toilet paper</t>
         </is>
       </c>
     </row>
     <row r="1693" ht="20" customHeight="1">
-      <c r="A1693" s="4" t="inlineStr">
+      <c r="A1693" s="3" t="inlineStr">
         <is>
           <t>Double bedrooms</t>
         </is>
       </c>
     </row>
     <row r="1694" ht="20" customHeight="1">
-      <c r="A1694" s="4" t="inlineStr">
+      <c r="A1694" s="3" t="inlineStr">
         <is>
           <t>En-suite bathroom</t>
         </is>
       </c>
     </row>
     <row r="1695" ht="20" customHeight="1">
-      <c r="A1695" s="4" t="inlineStr">
+      <c r="A1695" s="3" t="inlineStr">
         <is>
           <t>Hairdryer</t>
         </is>
       </c>
     </row>
     <row r="1696" ht="20" customHeight="1">
-      <c r="A1696" s="4" t="inlineStr">
+      <c r="A1696" s="3" t="inlineStr">
         <is>
           <t>Linen</t>
         </is>
       </c>
     </row>
     <row r="1697" ht="20" customHeight="1">
-      <c r="A1697" s="4" t="inlineStr">
+      <c r="A1697" s="3" t="inlineStr">
         <is>
           <t>Twin bedrooms</t>
         </is>
       </c>
     </row>
     <row r="1698" ht="31" customHeight="1">
-      <c r="A1698" s="14" t="inlineStr">
+      <c r="A1698" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve"> Outdoors</t>
         </is>
       </c>
     </row>
     <row r="1699" ht="20" customHeight="1">
-      <c r="A1699" s="4" t="inlineStr">
+      <c r="A1699" s="3" t="inlineStr">
         <is>
           <t>Barbecue</t>
         </is>
       </c>
     </row>
     <row r="1700" ht="20" customHeight="1">
-      <c r="A1700" s="4" t="inlineStr">
+      <c r="A1700" s="3" t="inlineStr">
         <is>
           <t>Deckchairs</t>
         </is>
       </c>
     </row>
     <row r="1701" ht="20" customHeight="1">
-      <c r="A1701" s="4" t="inlineStr">
+      <c r="A1701" s="3" t="inlineStr">
         <is>
           <t>Garden</t>
         </is>
       </c>
     </row>
     <row r="1702" ht="20" customHeight="1">
-      <c r="A1702" s="4" t="inlineStr">
+      <c r="A1702" s="3" t="inlineStr">
         <is>
           <t>Outdoor kitchen</t>
         </is>
       </c>
     </row>
     <row r="1703" ht="20" customHeight="1">
-      <c r="A1703" s="4" t="inlineStr">
+      <c r="A1703" s="3" t="inlineStr">
         <is>
           <t>Outdoor shower</t>
         </is>
       </c>
     </row>
     <row r="1704" ht="20" customHeight="1">
-      <c r="A1704" s="4" t="inlineStr">
+      <c r="A1704" s="3" t="inlineStr">
         <is>
           <t>Private parking</t>
         </is>
       </c>
     </row>
     <row r="1705" ht="20" customHeight="1">
-      <c r="A1705" s="4" t="inlineStr">
+      <c r="A1705" s="3" t="inlineStr">
         <is>
           <t>Private swimming pool</t>
         </is>
       </c>
     </row>
     <row r="1706" ht="20" customHeight="1">
-      <c r="A1706" s="4" t="inlineStr">
+      <c r="A1706" s="3" t="inlineStr">
         <is>
           <t>Terrace</t>
         </is>
       </c>
     </row>
     <row r="1707" ht="31" customHeight="1">
-      <c r="A1707" s="14" t="inlineStr">
+      <c r="A1707" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve"> Other amenities</t>
         </is>
       </c>
     </row>
     <row r="1708" ht="20" customHeight="1">
-      <c r="A1708" s="4" t="inlineStr">
+      <c r="A1708" s="3" t="inlineStr">
         <is>
           <t>Air conditioning</t>
         </is>
       </c>
     </row>
     <row r="1709" ht="20" customHeight="1">
-      <c r="A1709" s="4" t="inlineStr">
+      <c r="A1709" s="3" t="inlineStr">
         <is>
           <t>Beach umbrella and chairs</t>
         </is>
       </c>
     </row>
     <row r="1710" ht="20" customHeight="1">
-      <c r="A1710" s="4" t="inlineStr">
+      <c r="A1710" s="3" t="inlineStr">
         <is>
           <t>Board games</t>
         </is>
       </c>
     </row>
     <row r="1711" ht="20" customHeight="1">
-      <c r="A1711" s="4" t="inlineStr">
+      <c r="A1711" s="3" t="inlineStr">
         <is>
           <t>Canoe</t>
         </is>
       </c>
     </row>
     <row r="1712" ht="20" customHeight="1">
-      <c r="A1712" s="4" t="inlineStr">
+      <c r="A1712" s="3" t="inlineStr">
         <is>
           <t>Central heating</t>
         </is>
       </c>
     </row>
     <row r="1713" ht="20" customHeight="1">
-      <c r="A1713" s="4" t="inlineStr">
+      <c r="A1713" s="3" t="inlineStr">
         <is>
           <t>Electric vehicle charger</t>
         </is>
       </c>
     </row>
     <row r="1714" ht="20" customHeight="1">
-      <c r="A1714" s="4" t="inlineStr">
+      <c r="A1714" s="3" t="inlineStr">
         <is>
           <t>Highchair</t>
         </is>
       </c>
     </row>
     <row r="1715" ht="20" customHeight="1">
-      <c r="A1715" s="4" t="inlineStr">
+      <c r="A1715" s="3" t="inlineStr">
         <is>
           <t>Insect repellents</t>
         </is>
       </c>
     </row>
     <row r="1716" ht="20" customHeight="1">
-      <c r="A1716" s="4" t="inlineStr">
+      <c r="A1716" s="3" t="inlineStr">
         <is>
           <t>Internet Wi-Fi</t>
         </is>
       </c>
     </row>
     <row r="1717" ht="20" customHeight="1">
-      <c r="A1717" s="4" t="inlineStr">
+      <c r="A1717" s="3" t="inlineStr">
         <is>
           <t>Non-smoking</t>
         </is>
       </c>
     </row>
     <row r="1718" ht="20" customHeight="1">
-      <c r="A1718" s="4" t="inlineStr">
+      <c r="A1718" s="3" t="inlineStr">
         <is>
           <t>Pay per view (Sky, Netflix or Premium)</t>
         </is>
       </c>
     </row>
     <row r="1719" ht="20" customHeight="1">
-      <c r="A1719" s="4" t="inlineStr">
+      <c r="A1719" s="3" t="inlineStr">
         <is>
           <t>Ping pong table</t>
         </is>
       </c>
     </row>
     <row r="1720" ht="20" customHeight="1">
-      <c r="A1720" s="4" t="inlineStr">
+      <c r="A1720" s="3" t="inlineStr">
         <is>
           <t>Pool towels</t>
         </is>
       </c>
     </row>
     <row r="1721" ht="20" customHeight="1">
-      <c r="A1721" s="4" t="inlineStr">
+      <c r="A1721" s="3" t="inlineStr">
         <is>
           <t>Rowing Boat</t>
         </is>
       </c>
     </row>
     <row r="1722" ht="20" customHeight="1">
-      <c r="A1722" s="4" t="inlineStr">
+      <c r="A1722" s="3" t="inlineStr">
         <is>
           <t>Weekly cleaning</t>
         </is>
       </c>
     </row>
     <row r="1723" ht="20" customHeight="1">
-      <c r="A1723" s="4" t="inlineStr">
+      <c r="A1723" s="3" t="inlineStr">
         <is>
           <t>Welcome hamper</t>
         </is>
@@ -7436,84 +7169,84 @@
       </c>
     </row>
     <row r="1726" ht="31" customHeight="1">
-      <c r="A1726" s="14" t="inlineStr">
+      <c r="A1726" s="13" t="inlineStr">
         <is>
           <t>Good to know</t>
         </is>
       </c>
     </row>
     <row r="1728" ht="34" customHeight="1">
-      <c r="A1728" s="16" t="inlineStr">
+      <c r="A1728" s="15" t="inlineStr">
         <is>
           <t>infoHow to pay for your stayproperty listing</t>
         </is>
       </c>
     </row>
     <row r="1729" ht="34" customHeight="1">
-      <c r="A1729" s="16" t="inlineStr">
+      <c r="A1729" s="15" t="inlineStr">
         <is>
           <t>checkAdditional notesand house rules</t>
         </is>
       </c>
     </row>
     <row r="1730" ht="34" customHeight="1">
-      <c r="A1730" s="16" t="inlineStr">
+      <c r="A1730" s="15" t="inlineStr">
         <is>
           <t>room_serviceExtra costsand what to pay upon arrival</t>
         </is>
       </c>
     </row>
     <row r="1731" ht="34" customHeight="1">
-      <c r="A1731" s="16" t="inlineStr">
+      <c r="A1731" s="15" t="inlineStr">
         <is>
           <t>boltSicily Experiences TrioSave on a package of 3 Active Experiences</t>
         </is>
       </c>
     </row>
     <row r="1732" ht="31" customHeight="1">
-      <c r="A1732" s="14" t="inlineStr">
+      <c r="A1732" s="13" t="inlineStr">
         <is>
           <t>Area</t>
         </is>
       </c>
     </row>
     <row r="1734" ht="20" customHeight="1">
-      <c r="A1734" s="4" t="inlineStr">
+      <c r="A1734" s="3" t="inlineStr">
         <is>
           <t>This unique beachfront villa is located a short drive from Finale di Pollina (2km), a charming seaside village on the north coast of Sicily, where you can get everything you need from a good selection of shops, restaurants, trattorie, pizzerie and bars. The beach is literally on your doorstep and the panoramic terrace enjoys a splendid view of the whole coast.</t>
         </is>
       </c>
     </row>
     <row r="1736" ht="20" customHeight="1">
-      <c r="A1736" s="4" t="inlineStr">
+      <c r="A1736" s="3" t="inlineStr">
         <is>
           <t>A quick 15-minute motorway drive takes you to the seaside resort of Cefalù. This is one of Sicily’s busier towns, particularly during the summer months, thanks to its fish restaurants, shops and fabulous beaches. However, a visit here is enjoyable at any time of year thanks to its UNESCO world heritage Norman cathedral and its medieval town centre. Banks, shops and supermarkets are all available here. Continuing west along the coast, you reach Palermo (just over an hour) where there are some superb sightseeing opportunities and, of course, the city’s famous street food markets.</t>
         </is>
       </c>
     </row>
     <row r="1738" ht="20" customHeight="1">
-      <c r="A1738" s="4" t="inlineStr">
+      <c r="A1738" s="3" t="inlineStr">
         <is>
           <t>If you like the idea of leaving the car behind and hopping on a train, the recently opened Finale di Pollina railway station is just 5 minutes’ walk away. The small electric train connects a series of towns along Sicily’s north coast, from Palermo to Messina and including Cefalu. Despite the proximity to the station, the train can barely be heard.</t>
         </is>
       </c>
     </row>
     <row r="1740" ht="20" customHeight="1">
-      <c r="A1740" s="4" t="inlineStr">
+      <c r="A1740" s="3" t="inlineStr">
         <is>
           <t>A little further afield, though little more than an hour away, the Greek temple and theatre at Segesta is well worth a visit. Other local archaeological sites include Himera which is less than 40 minutes by car. If you feel like getting right off the beaten track, the Madonie National Park is a glorious spot for hiking, great views or exploring medieval hilltop towns such as Polizzi Generosa or Petralia Soprana.</t>
         </is>
       </c>
     </row>
     <row r="1742" ht="20" customHeight="1">
-      <c r="A1742" s="4" t="inlineStr">
+      <c r="A1742" s="3" t="inlineStr">
         <is>
           <t>A brand-new spot has just opened in Costa Turchina: Beach Club Costa Turchina, a laid-back restaurant and lounge bar. It's just a short walk from the villa, making it easy to enjoy a pizza, a seafood dinner, or a relaxed drink in the evening. Additionally, the Beach Club offers rentals of electric bikes, scooters, and boats, so you can explore the area with complete freedom. A great addition to make your stay even more enjoyable!</t>
         </is>
       </c>
     </row>
     <row r="1744" ht="20" customHeight="1">
-      <c r="A1744" s="15" t="inlineStr">
+      <c r="A1744" s="14" t="inlineStr">
         <is>
           <t>read more</t>
         </is>
@@ -7527,42 +7260,42 @@
       </c>
     </row>
     <row r="1746" ht="19" customHeight="1">
-      <c r="A1746" s="17" t="inlineStr">
+      <c r="A1746" s="16" t="inlineStr">
         <is>
           <t>5 (5 Reviews)</t>
         </is>
       </c>
     </row>
     <row r="1747" ht="18" customHeight="1">
-      <c r="A1747" s="18" t="inlineStr">
+      <c r="A1747" s="17" t="inlineStr">
         <is>
           <t>Check-inpick a dateCheck-outpick a date</t>
         </is>
       </c>
     </row>
     <row r="1748" ht="20" customHeight="1">
-      <c r="A1748" s="15" t="inlineStr">
+      <c r="A1748" s="14" t="inlineStr">
         <is>
           <t>Guests0 adult 0 child 0 infant 0 pet</t>
         </is>
       </c>
     </row>
     <row r="1749" ht="20" customHeight="1">
-      <c r="A1749" s="15" t="inlineStr">
+      <c r="A1749" s="14" t="inlineStr">
         <is>
           <t>Bedrooms0 bedroom</t>
         </is>
       </c>
     </row>
     <row r="1750" ht="18" customHeight="1">
-      <c r="A1750" s="19" t="inlineStr">
+      <c r="A1750" s="18" t="inlineStr">
         <is>
           <t>Price per night from€ 260.00</t>
         </is>
       </c>
     </row>
     <row r="1751" ht="23" customHeight="1">
-      <c r="A1751" s="20" t="inlineStr">
+      <c r="A1751" s="19" t="inlineStr">
         <is>
           <t>Book online</t>
         </is>
@@ -7576,497 +7309,497 @@
       </c>
     </row>
     <row r="1753" ht="100" customHeight="1">
-      <c r="A1753" s="21" t="inlineStr">
+      <c r="A1753" s="20" t="inlineStr">
         <is>
           <t>Discover</t>
         </is>
       </c>
     </row>
     <row r="1755" ht="20" customHeight="1">
-      <c r="A1755" s="4" t="inlineStr">
+      <c r="A1755" s="3" t="inlineStr">
         <is>
           <t>Discover places of interest and services near Aqua Turchina</t>
         </is>
       </c>
     </row>
     <row r="1757" ht="20" customHeight="1">
-      <c r="A1757" s="15" t="inlineStr">
+      <c r="A1757" s="14" t="inlineStr">
         <is>
           <t>Food</t>
         </is>
       </c>
     </row>
     <row r="1758" ht="20" customHeight="1">
-      <c r="A1758" s="15" t="inlineStr">
+      <c r="A1758" s="14" t="inlineStr">
         <is>
           <t>Health</t>
         </is>
       </c>
     </row>
     <row r="1759" ht="20" customHeight="1">
-      <c r="A1759" s="15" t="inlineStr">
+      <c r="A1759" s="14" t="inlineStr">
         <is>
           <t>Amenities</t>
         </is>
       </c>
     </row>
     <row r="1760" ht="20" customHeight="1">
-      <c r="A1760" s="15" t="inlineStr">
+      <c r="A1760" s="14" t="inlineStr">
         <is>
           <t>Tourist attractions</t>
         </is>
       </c>
     </row>
     <row r="1761" ht="20" customHeight="1">
-      <c r="A1761" s="15" t="inlineStr">
+      <c r="A1761" s="14" t="inlineStr">
         <is>
           <t>Reset</t>
         </is>
       </c>
     </row>
     <row r="1762">
-      <c r="A1762" s="22" t="n"/>
+      <c r="A1762" s="21" t="n"/>
     </row>
     <row r="1763">
-      <c r="A1763" s="22" t="n"/>
+      <c r="A1763" s="21" t="n"/>
     </row>
     <row r="1764">
-      <c r="A1764" s="22" t="n"/>
+      <c r="A1764" s="21" t="n"/>
     </row>
     <row r="1765">
-      <c r="A1765" s="22" t="n"/>
+      <c r="A1765" s="21" t="n"/>
     </row>
     <row r="1766">
-      <c r="A1766" s="22" t="n"/>
+      <c r="A1766" s="21" t="n"/>
     </row>
     <row r="1767">
-      <c r="A1767" s="22" t="n"/>
+      <c r="A1767" s="21" t="n"/>
     </row>
     <row r="1768">
-      <c r="A1768" s="22" t="n"/>
+      <c r="A1768" s="21" t="n"/>
     </row>
     <row r="1769">
-      <c r="A1769" s="22" t="n"/>
+      <c r="A1769" s="21" t="n"/>
     </row>
     <row r="1770">
-      <c r="A1770" s="22" t="n"/>
+      <c r="A1770" s="21" t="n"/>
     </row>
     <row r="1771">
-      <c r="A1771" s="22" t="n"/>
+      <c r="A1771" s="21" t="n"/>
     </row>
     <row r="1772">
-      <c r="A1772" s="22" t="n"/>
+      <c r="A1772" s="21" t="n"/>
     </row>
     <row r="1773">
-      <c r="A1773" s="22" t="n"/>
+      <c r="A1773" s="21" t="n"/>
     </row>
     <row r="1774">
-      <c r="A1774" s="22" t="n"/>
+      <c r="A1774" s="21" t="n"/>
     </row>
     <row r="1775">
-      <c r="A1775" s="22" t="n"/>
+      <c r="A1775" s="21" t="n"/>
     </row>
     <row r="1776">
-      <c r="A1776" s="22" t="n"/>
+      <c r="A1776" s="21" t="n"/>
     </row>
     <row r="1777">
-      <c r="A1777" s="22" t="n"/>
+      <c r="A1777" s="21" t="n"/>
     </row>
     <row r="1778">
-      <c r="A1778" s="22" t="n"/>
+      <c r="A1778" s="21" t="n"/>
     </row>
     <row r="1779">
-      <c r="A1779" s="22" t="n"/>
+      <c r="A1779" s="21" t="n"/>
     </row>
     <row r="1780">
-      <c r="A1780" s="22" t="n"/>
+      <c r="A1780" s="21" t="n"/>
     </row>
     <row r="1781">
-      <c r="A1781" s="22" t="n"/>
+      <c r="A1781" s="21" t="n"/>
     </row>
     <row r="1782">
-      <c r="A1782" s="22" t="n"/>
+      <c r="A1782" s="21" t="n"/>
     </row>
     <row r="1783">
-      <c r="A1783" s="22" t="n"/>
+      <c r="A1783" s="21" t="n"/>
     </row>
     <row r="1784">
-      <c r="A1784" s="22" t="n"/>
+      <c r="A1784" s="21" t="n"/>
     </row>
     <row r="1785">
-      <c r="A1785" s="22" t="n"/>
+      <c r="A1785" s="21" t="n"/>
     </row>
     <row r="1786">
-      <c r="A1786" s="22" t="n"/>
+      <c r="A1786" s="21" t="n"/>
     </row>
     <row r="1787">
-      <c r="A1787" s="22" t="n"/>
+      <c r="A1787" s="21" t="n"/>
     </row>
     <row r="1788">
-      <c r="A1788" s="22" t="n"/>
+      <c r="A1788" s="21" t="n"/>
     </row>
     <row r="1789">
-      <c r="A1789" s="22" t="n"/>
+      <c r="A1789" s="21" t="n"/>
     </row>
     <row r="1790">
-      <c r="A1790" s="22" t="n"/>
+      <c r="A1790" s="21" t="n"/>
     </row>
     <row r="1791">
-      <c r="A1791" s="22" t="n"/>
+      <c r="A1791" s="21" t="n"/>
     </row>
     <row r="1792">
-      <c r="A1792" s="22" t="n"/>
+      <c r="A1792" s="21" t="n"/>
     </row>
     <row r="1793">
-      <c r="A1793" s="22" t="n"/>
+      <c r="A1793" s="21" t="n"/>
     </row>
     <row r="1794">
-      <c r="A1794" s="22" t="n"/>
+      <c r="A1794" s="21" t="n"/>
     </row>
     <row r="1795">
-      <c r="A1795" s="22" t="n"/>
+      <c r="A1795" s="21" t="n"/>
     </row>
     <row r="1796">
-      <c r="A1796" s="22" t="n"/>
+      <c r="A1796" s="21" t="n"/>
     </row>
     <row r="1797">
-      <c r="A1797" s="22" t="n"/>
+      <c r="A1797" s="21" t="n"/>
     </row>
     <row r="1798">
-      <c r="A1798" s="22" t="n"/>
+      <c r="A1798" s="21" t="n"/>
     </row>
     <row r="1799">
-      <c r="A1799" s="22" t="n"/>
+      <c r="A1799" s="21" t="n"/>
     </row>
     <row r="1800">
-      <c r="A1800" s="22" t="n"/>
+      <c r="A1800" s="21" t="n"/>
     </row>
     <row r="1801">
-      <c r="A1801" s="22" t="n"/>
+      <c r="A1801" s="21" t="n"/>
     </row>
     <row r="1802">
-      <c r="A1802" s="22" t="n"/>
+      <c r="A1802" s="21" t="n"/>
     </row>
     <row r="1803">
-      <c r="A1803" s="22" t="n"/>
+      <c r="A1803" s="21" t="n"/>
     </row>
     <row r="1804">
-      <c r="A1804" s="22" t="n"/>
+      <c r="A1804" s="21" t="n"/>
     </row>
     <row r="1805">
-      <c r="A1805" s="22" t="n"/>
+      <c r="A1805" s="21" t="n"/>
     </row>
     <row r="1806">
-      <c r="A1806" s="22" t="n"/>
+      <c r="A1806" s="21" t="n"/>
     </row>
     <row r="1807">
-      <c r="A1807" s="22" t="n"/>
+      <c r="A1807" s="21" t="n"/>
     </row>
     <row r="1808">
-      <c r="A1808" s="22" t="n"/>
+      <c r="A1808" s="21" t="n"/>
     </row>
     <row r="1809">
-      <c r="A1809" s="22" t="n"/>
+      <c r="A1809" s="21" t="n"/>
     </row>
     <row r="1810">
-      <c r="A1810" s="22" t="n"/>
+      <c r="A1810" s="21" t="n"/>
     </row>
     <row r="1811">
-      <c r="A1811" s="22" t="n"/>
+      <c r="A1811" s="21" t="n"/>
     </row>
     <row r="1812">
-      <c r="A1812" s="22" t="n"/>
+      <c r="A1812" s="21" t="n"/>
     </row>
     <row r="1813">
-      <c r="A1813" s="22" t="n"/>
+      <c r="A1813" s="21" t="n"/>
     </row>
     <row r="1814">
-      <c r="A1814" s="22" t="n"/>
+      <c r="A1814" s="21" t="n"/>
     </row>
     <row r="1815">
-      <c r="A1815" s="22" t="n"/>
+      <c r="A1815" s="21" t="n"/>
     </row>
     <row r="1816">
-      <c r="A1816" s="22" t="n"/>
+      <c r="A1816" s="21" t="n"/>
     </row>
     <row r="1817">
-      <c r="A1817" s="22" t="n"/>
+      <c r="A1817" s="21" t="n"/>
     </row>
     <row r="1818">
-      <c r="A1818" s="22" t="n"/>
+      <c r="A1818" s="21" t="n"/>
     </row>
     <row r="1819">
-      <c r="A1819" s="22" t="n"/>
+      <c r="A1819" s="21" t="n"/>
     </row>
     <row r="1820">
-      <c r="A1820" s="22" t="n"/>
+      <c r="A1820" s="21" t="n"/>
     </row>
     <row r="1821">
-      <c r="A1821" s="22" t="n"/>
+      <c r="A1821" s="21" t="n"/>
     </row>
     <row r="1822">
-      <c r="A1822" s="22" t="n"/>
+      <c r="A1822" s="21" t="n"/>
     </row>
     <row r="1823">
-      <c r="A1823" s="22" t="n"/>
+      <c r="A1823" s="21" t="n"/>
     </row>
     <row r="1824">
-      <c r="A1824" s="22" t="n"/>
+      <c r="A1824" s="21" t="n"/>
     </row>
     <row r="1825">
-      <c r="A1825" s="22" t="n"/>
+      <c r="A1825" s="21" t="n"/>
     </row>
     <row r="1826">
-      <c r="A1826" s="22" t="n"/>
+      <c r="A1826" s="21" t="n"/>
     </row>
     <row r="1827">
-      <c r="A1827" s="22" t="n"/>
+      <c r="A1827" s="21" t="n"/>
     </row>
     <row r="1828">
-      <c r="A1828" s="22" t="n"/>
+      <c r="A1828" s="21" t="n"/>
     </row>
     <row r="1829">
-      <c r="A1829" s="22" t="n"/>
+      <c r="A1829" s="21" t="n"/>
     </row>
     <row r="1830">
-      <c r="A1830" s="22" t="n"/>
+      <c r="A1830" s="21" t="n"/>
     </row>
     <row r="1831">
-      <c r="A1831" s="22" t="n"/>
+      <c r="A1831" s="21" t="n"/>
     </row>
     <row r="1832">
-      <c r="A1832" s="22" t="n"/>
+      <c r="A1832" s="21" t="n"/>
     </row>
     <row r="1833">
-      <c r="A1833" s="22" t="n"/>
+      <c r="A1833" s="21" t="n"/>
     </row>
     <row r="1834">
-      <c r="A1834" s="22" t="n"/>
+      <c r="A1834" s="21" t="n"/>
     </row>
     <row r="1835">
-      <c r="A1835" s="22" t="n"/>
+      <c r="A1835" s="21" t="n"/>
     </row>
     <row r="1836">
-      <c r="A1836" s="22" t="n"/>
+      <c r="A1836" s="21" t="n"/>
     </row>
     <row r="1837">
-      <c r="A1837" s="22" t="n"/>
+      <c r="A1837" s="21" t="n"/>
     </row>
     <row r="1838">
-      <c r="A1838" s="22" t="n"/>
+      <c r="A1838" s="21" t="n"/>
     </row>
     <row r="1839">
-      <c r="A1839" s="22" t="n"/>
+      <c r="A1839" s="21" t="n"/>
     </row>
     <row r="1840">
-      <c r="A1840" s="22" t="n"/>
+      <c r="A1840" s="21" t="n"/>
     </row>
     <row r="1841">
-      <c r="A1841" s="22" t="n"/>
+      <c r="A1841" s="21" t="n"/>
     </row>
     <row r="1842">
-      <c r="A1842" s="22" t="n"/>
+      <c r="A1842" s="21" t="n"/>
     </row>
     <row r="1843">
-      <c r="A1843" s="22" t="n"/>
+      <c r="A1843" s="21" t="n"/>
     </row>
     <row r="1844">
-      <c r="A1844" s="22" t="n"/>
+      <c r="A1844" s="21" t="n"/>
     </row>
     <row r="1845">
-      <c r="A1845" s="22" t="n"/>
+      <c r="A1845" s="21" t="n"/>
     </row>
     <row r="1846">
-      <c r="A1846" s="22" t="n"/>
+      <c r="A1846" s="21" t="n"/>
     </row>
     <row r="1847">
-      <c r="A1847" s="22" t="n"/>
+      <c r="A1847" s="21" t="n"/>
     </row>
     <row r="1848">
-      <c r="A1848" s="22" t="n"/>
+      <c r="A1848" s="21" t="n"/>
     </row>
     <row r="1849">
-      <c r="A1849" s="22" t="n"/>
+      <c r="A1849" s="21" t="n"/>
     </row>
     <row r="1850">
-      <c r="A1850" s="22" t="n"/>
+      <c r="A1850" s="21" t="n"/>
     </row>
     <row r="1851">
-      <c r="A1851" s="22" t="n"/>
+      <c r="A1851" s="21" t="n"/>
     </row>
     <row r="1852">
-      <c r="A1852" s="22" t="n"/>
+      <c r="A1852" s="21" t="n"/>
     </row>
     <row r="1853">
-      <c r="A1853" s="22" t="n"/>
+      <c r="A1853" s="21" t="n"/>
     </row>
     <row r="1854">
-      <c r="A1854" s="22" t="n"/>
+      <c r="A1854" s="21" t="n"/>
     </row>
     <row r="1855">
-      <c r="A1855" s="22" t="n"/>
+      <c r="A1855" s="21" t="n"/>
     </row>
     <row r="1856">
-      <c r="A1856" s="22" t="n"/>
+      <c r="A1856" s="21" t="n"/>
     </row>
     <row r="1857">
-      <c r="A1857" s="22" t="n"/>
+      <c r="A1857" s="21" t="n"/>
     </row>
     <row r="1858">
-      <c r="A1858" s="22" t="n"/>
+      <c r="A1858" s="21" t="n"/>
     </row>
     <row r="1859">
-      <c r="A1859" s="22" t="n"/>
+      <c r="A1859" s="21" t="n"/>
     </row>
     <row r="1860">
-      <c r="A1860" s="22" t="n"/>
+      <c r="A1860" s="21" t="n"/>
     </row>
     <row r="1861">
-      <c r="A1861" s="22" t="n"/>
+      <c r="A1861" s="21" t="n"/>
     </row>
     <row r="1862">
-      <c r="A1862" s="22" t="n"/>
+      <c r="A1862" s="21" t="n"/>
     </row>
     <row r="1863">
-      <c r="A1863" s="22" t="n"/>
+      <c r="A1863" s="21" t="n"/>
     </row>
     <row r="1864">
-      <c r="A1864" s="22" t="n"/>
+      <c r="A1864" s="21" t="n"/>
     </row>
     <row r="1865">
-      <c r="A1865" s="22" t="n"/>
+      <c r="A1865" s="21" t="n"/>
     </row>
     <row r="1866">
-      <c r="A1866" s="22" t="n"/>
+      <c r="A1866" s="21" t="n"/>
     </row>
     <row r="1867">
-      <c r="A1867" s="22" t="n"/>
+      <c r="A1867" s="21" t="n"/>
     </row>
     <row r="1868">
-      <c r="A1868" s="22" t="n"/>
+      <c r="A1868" s="21" t="n"/>
     </row>
     <row r="1869">
-      <c r="A1869" s="22" t="n"/>
+      <c r="A1869" s="21" t="n"/>
     </row>
     <row r="1870">
-      <c r="A1870" s="22" t="n"/>
+      <c r="A1870" s="21" t="n"/>
     </row>
     <row r="1871">
-      <c r="A1871" s="22" t="n"/>
+      <c r="A1871" s="21" t="n"/>
     </row>
     <row r="1872">
-      <c r="A1872" s="22" t="n"/>
+      <c r="A1872" s="21" t="n"/>
     </row>
     <row r="1873">
-      <c r="A1873" s="22" t="n"/>
+      <c r="A1873" s="21" t="n"/>
     </row>
     <row r="1874">
-      <c r="A1874" s="22" t="n"/>
+      <c r="A1874" s="21" t="n"/>
     </row>
     <row r="1875">
-      <c r="A1875" s="22" t="n"/>
+      <c r="A1875" s="21" t="n"/>
     </row>
     <row r="1876">
-      <c r="A1876" s="22" t="n"/>
+      <c r="A1876" s="21" t="n"/>
     </row>
     <row r="1877">
-      <c r="A1877" s="22" t="n"/>
+      <c r="A1877" s="21" t="n"/>
     </row>
     <row r="1878">
-      <c r="A1878" s="22" t="n"/>
+      <c r="A1878" s="21" t="n"/>
     </row>
     <row r="1879">
-      <c r="A1879" s="22" t="n"/>
+      <c r="A1879" s="21" t="n"/>
     </row>
     <row r="1880">
-      <c r="A1880" s="22" t="n"/>
+      <c r="A1880" s="21" t="n"/>
     </row>
     <row r="1881">
-      <c r="A1881" s="22" t="n"/>
+      <c r="A1881" s="21" t="n"/>
     </row>
     <row r="1882" ht="34" customHeight="1">
-      <c r="A1882" s="23" t="inlineStr">
+      <c r="A1882" s="22" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
     </row>
     <row r="1883" ht="34" customHeight="1">
-      <c r="A1883" s="23" t="inlineStr">
+      <c r="A1883" s="22" t="inlineStr">
         <is>
           <t>remove</t>
         </is>
       </c>
     </row>
     <row r="1884" ht="20" customHeight="1">
-      <c r="A1884" s="11" t="n"/>
+      <c r="A1884" s="10" t="n"/>
     </row>
     <row r="1885" ht="100" customHeight="1">
-      <c r="A1885" s="21" t="inlineStr">
+      <c r="A1885" s="20" t="inlineStr">
         <is>
           <t>Surroundings</t>
         </is>
       </c>
     </row>
     <row r="1887" ht="148" customHeight="1">
-      <c r="A1887" s="24" t="inlineStr">
+      <c r="A1887" s="23" t="inlineStr">
         <is>
           <t>Cefalù</t>
         </is>
       </c>
     </row>
     <row r="1888" ht="20" customHeight="1">
-      <c r="A1888" s="11" t="n"/>
+      <c r="A1888" s="10" t="n"/>
     </row>
     <row r="1889" ht="20" customHeight="1">
-      <c r="A1889" s="11" t="n"/>
+      <c r="A1889" s="10" t="n"/>
     </row>
     <row r="1890" ht="20" customHeight="1">
-      <c r="A1890" s="11" t="n"/>
+      <c r="A1890" s="10" t="n"/>
     </row>
     <row r="1891" ht="20" customHeight="1">
-      <c r="A1891" s="11" t="n"/>
+      <c r="A1891" s="10" t="n"/>
     </row>
     <row r="1892" ht="20" customHeight="1">
-      <c r="A1892" s="11" t="n"/>
+      <c r="A1892" s="10" t="n"/>
     </row>
     <row r="1893" ht="20" customHeight="1">
-      <c r="A1893" s="11" t="n"/>
+      <c r="A1893" s="10" t="n"/>
     </row>
     <row r="1894" ht="20" customHeight="1">
-      <c r="A1894" s="11" t="n"/>
+      <c r="A1894" s="10" t="n"/>
     </row>
     <row r="1895" ht="20" customHeight="1">
-      <c r="A1895" s="11" t="n"/>
+      <c r="A1895" s="10" t="n"/>
     </row>
     <row r="1896" ht="20" customHeight="1">
-      <c r="A1896" s="11" t="n"/>
+      <c r="A1896" s="10" t="n"/>
     </row>
     <row r="1897" ht="20" customHeight="1">
-      <c r="A1897" s="11" t="n"/>
+      <c r="A1897" s="10" t="n"/>
     </row>
     <row r="1898" ht="20" customHeight="1">
-      <c r="A1898" s="11" t="n"/>
+      <c r="A1898" s="10" t="n"/>
     </row>
     <row r="1899" ht="20" customHeight="1">
-      <c r="A1899" s="11" t="n"/>
+      <c r="A1899" s="10" t="n"/>
     </row>
     <row r="1900" ht="100" customHeight="1">
-      <c r="A1900" s="21" t="inlineStr">
+      <c r="A1900" s="20" t="inlineStr">
         <is>
           <t>Experiences</t>
         </is>
       </c>
     </row>
     <row r="1902" ht="20" customHeight="1">
-      <c r="A1902" s="4" t="inlineStr">
+      <c r="A1902" s="3" t="inlineStr">
         <is>
           <t>Book one of our Experiences with Aqua Turchina</t>
         </is>
       </c>
     </row>
     <row r="1904" ht="20" customHeight="1">
-      <c r="A1904" s="4" t="n"/>
+      <c r="A1904" s="3" t="n"/>
     </row>
     <row r="1906">
       <c r="A1906" s="1" t="inlineStr">
@@ -8076,72 +7809,72 @@
       </c>
     </row>
     <row r="1907" ht="20" customHeight="1">
-      <c r="A1907" s="11" t="n"/>
+      <c r="A1907" s="10" t="n"/>
     </row>
     <row r="1908" ht="20" customHeight="1">
-      <c r="A1908" s="11" t="n"/>
+      <c r="A1908" s="10" t="n"/>
     </row>
     <row r="1909" ht="20" customHeight="1">
-      <c r="A1909" s="11" t="n"/>
+      <c r="A1909" s="10" t="n"/>
     </row>
     <row r="1910" ht="20" customHeight="1">
-      <c r="A1910" s="11" t="n"/>
+      <c r="A1910" s="10" t="n"/>
     </row>
     <row r="1911" ht="20" customHeight="1">
-      <c r="A1911" s="11" t="n"/>
+      <c r="A1911" s="10" t="n"/>
     </row>
     <row r="1912" ht="20" customHeight="1">
-      <c r="A1912" s="11" t="n"/>
+      <c r="A1912" s="10" t="n"/>
     </row>
     <row r="1913" ht="20" customHeight="1">
-      <c r="A1913" s="11" t="n"/>
+      <c r="A1913" s="10" t="n"/>
     </row>
     <row r="1914" ht="20" customHeight="1">
-      <c r="A1914" s="11" t="n"/>
+      <c r="A1914" s="10" t="n"/>
     </row>
     <row r="1915" ht="20" customHeight="1">
-      <c r="A1915" s="11" t="n"/>
+      <c r="A1915" s="10" t="n"/>
     </row>
     <row r="1916" ht="20" customHeight="1">
-      <c r="A1916" s="11" t="n"/>
+      <c r="A1916" s="10" t="n"/>
     </row>
     <row r="1917" ht="20" customHeight="1">
-      <c r="A1917" s="11" t="n"/>
+      <c r="A1917" s="10" t="n"/>
     </row>
     <row r="1918" ht="20" customHeight="1">
-      <c r="A1918" s="11" t="n"/>
+      <c r="A1918" s="10" t="n"/>
     </row>
     <row r="1919" ht="20" customHeight="1">
-      <c r="A1919" s="11" t="n"/>
+      <c r="A1919" s="10" t="n"/>
     </row>
     <row r="1920" ht="20" customHeight="1">
-      <c r="A1920" s="11" t="n"/>
+      <c r="A1920" s="10" t="n"/>
     </row>
     <row r="1921" ht="20" customHeight="1">
-      <c r="A1921" s="11" t="n"/>
+      <c r="A1921" s="10" t="n"/>
     </row>
     <row r="1922" ht="20" customHeight="1">
-      <c r="A1922" s="11" t="n"/>
+      <c r="A1922" s="10" t="n"/>
     </row>
     <row r="1923" ht="100" customHeight="1">
-      <c r="A1923" s="21" t="inlineStr">
+      <c r="A1923" s="20" t="inlineStr">
         <is>
           <t>Press</t>
         </is>
       </c>
     </row>
     <row r="1925" ht="20" customHeight="1">
-      <c r="A1925" s="4" t="inlineStr">
+      <c r="A1925" s="3" t="inlineStr">
         <is>
           <t>Aqua Turchina appeared on these articles</t>
         </is>
       </c>
     </row>
     <row r="1926" ht="20" customHeight="1">
-      <c r="A1926" s="11" t="n"/>
+      <c r="A1926" s="10" t="n"/>
     </row>
     <row r="1927" ht="20" customHeight="1">
-      <c r="A1927" s="11" t="n"/>
+      <c r="A1927" s="10" t="n"/>
     </row>
     <row r="1928">
       <c r="A1928" s="1" t="inlineStr">
@@ -8158,14 +7891,14 @@
       </c>
     </row>
     <row r="1930" ht="100" customHeight="1">
-      <c r="A1930" s="25" t="inlineStr">
+      <c r="A1930" s="24" t="inlineStr">
         <is>
           <t>Reviews</t>
         </is>
       </c>
     </row>
     <row r="1932" ht="25" customHeight="1">
-      <c r="A1932" s="26" t="inlineStr">
+      <c r="A1932" s="25" t="inlineStr">
         <is>
           <t>5/5 100% genuine</t>
         </is>
@@ -8179,298 +7912,298 @@
       </c>
     </row>
     <row r="1934" ht="31" customHeight="1">
-      <c r="A1934" s="14" t="inlineStr">
+      <c r="A1934" s="13" t="inlineStr">
         <is>
           <t>Trusted c.</t>
         </is>
       </c>
     </row>
     <row r="1935" ht="20" customHeight="1">
-      <c r="A1935" s="27" t="n">
+      <c r="A1935" s="26" t="n">
         <v>45597</v>
       </c>
     </row>
     <row r="1936" ht="23" customHeight="1">
-      <c r="A1936" s="28" t="inlineStr">
+      <c r="A1936" s="27" t="inlineStr">
         <is>
           <t>Excellent accommodation</t>
         </is>
       </c>
     </row>
     <row r="1938" ht="20" customHeight="1">
-      <c r="A1938" s="4" t="inlineStr">
+      <c r="A1938" s="3" t="inlineStr">
         <is>
           <t>Everything good. Excellent accommodation :) Very friendly</t>
         </is>
       </c>
     </row>
     <row r="1939" ht="31" customHeight="1">
-      <c r="A1939" s="14" t="inlineStr">
+      <c r="A1939" s="13" t="inlineStr">
         <is>
           <t>Roberto M.</t>
         </is>
       </c>
     </row>
     <row r="1940" ht="20" customHeight="1">
-      <c r="A1940" s="27" t="n">
+      <c r="A1940" s="26" t="n">
         <v>45536</v>
       </c>
     </row>
     <row r="1941" ht="20" customHeight="1">
-      <c r="A1941" s="4" t="inlineStr">
+      <c r="A1941" s="3" t="inlineStr">
         <is>
           <t>Il nostro soggiorno ad Aqua Turchina è stato davvero piacevole. L'agenzia si è dimostrata efficiente e disponibile, rispondendo prontamente a ogni richiesta. La villa è in una posizione fantastica, con accesso diretto al mare, e una terrazza che offre una bella vista. Avere la spiaggia così vicina è stato un grande vantaggio, e la breve distanza da Finale di Pollina ci ha permesso di visitare facilmente il paese. Un'esperienza che consigliamo per una vacanza rilassante. Il nostro soggiorno ad Aqua Turchina è stato davvero piacevole. L'agenzia si è dimostrata efficiente e disponibile, rispondendo prontamente a ogni richiesta. La villa è in una posizione fantastica, con accesso diretto al mare, e una terrazza che offre una bella vista. Avere la spiaggia così vicina è stato un grande vantaggio, e la breve distanza da Finale di Pollina ci ha permesso di visitare facilmente il paese. Un'esperienza che consigliamo per una vacanza rilassante.</t>
         </is>
       </c>
     </row>
     <row r="1942" ht="20" customHeight="1">
-      <c r="A1942" s="15" t="inlineStr">
+      <c r="A1942" s="14" t="inlineStr">
         <is>
           <t>read more</t>
         </is>
       </c>
     </row>
     <row r="1943" ht="31" customHeight="1">
-      <c r="A1943" s="14" t="inlineStr">
+      <c r="A1943" s="13" t="inlineStr">
         <is>
           <t>Natalie J.</t>
         </is>
       </c>
     </row>
     <row r="1944" ht="20" customHeight="1">
-      <c r="A1944" s="27" t="n">
+      <c r="A1944" s="26" t="n">
         <v>45505</v>
       </c>
     </row>
     <row r="1945" ht="20" customHeight="1">
-      <c r="A1945" s="4" t="inlineStr">
+      <c r="A1945" s="3" t="inlineStr">
         <is>
           <t>Perfect vacation spot when traveling with family of all ages! Very clean house with private beach access ☀️ Friendly host who helped with local recommendations and even walked us to our first dinner reservation. Would definitely recommend their beautiful home to anyone going to the area! One suggestion - Make sure you’re familiar with European appliances before arrival!</t>
         </is>
       </c>
     </row>
     <row r="1946" ht="20" customHeight="1">
-      <c r="A1946" s="15" t="inlineStr">
+      <c r="A1946" s="14" t="inlineStr">
         <is>
           <t>read more</t>
         </is>
       </c>
     </row>
     <row r="1947" ht="31" customHeight="1">
-      <c r="A1947" s="14" t="inlineStr">
+      <c r="A1947" s="13" t="inlineStr">
         <is>
           <t>Trusted c.</t>
         </is>
       </c>
     </row>
     <row r="1948" ht="20" customHeight="1">
-      <c r="A1948" s="27" t="n">
+      <c r="A1948" s="26" t="n">
         <v>45474</v>
       </c>
     </row>
     <row r="1949" ht="23" customHeight="1">
-      <c r="A1949" s="28" t="inlineStr">
+      <c r="A1949" s="27" t="inlineStr">
         <is>
           <t>HOLIDAY WEEK IN FINALE DI POLLINA</t>
         </is>
       </c>
     </row>
     <row r="1951" ht="20" customHeight="1">
-      <c r="A1951" s="4" t="inlineStr">
+      <c r="A1951" s="3" t="inlineStr">
         <is>
           <t>PERFECT ACCOMODATION IN FRONT OF STUNNING SEA BEAUTIFUL HOUSE WITH ALL NEEDED AMENITIES NICE GARDEN AND POOL SPECIAL THANKS TO MR FRANCESCO ( OWNER OF THE HOUSE ) THAT WAS ALWAYS AVAILABLE AND REACHABLE FOR ALL OUR NEED AND INFORMATION TRYING TO SATISFY ALL OUR NEEDED AND REQUEST VERY HELPFUL AND ALWAYS AVAILABLE FOR ALL OUR RQUEST AND SUPPORT NEEDED</t>
         </is>
       </c>
     </row>
     <row r="1952" ht="20" customHeight="1">
-      <c r="A1952" s="15" t="inlineStr">
+      <c r="A1952" s="14" t="inlineStr">
         <is>
           <t>read more</t>
         </is>
       </c>
     </row>
     <row r="1953" ht="31" customHeight="1">
-      <c r="A1953" s="14" t="inlineStr">
+      <c r="A1953" s="13" t="inlineStr">
         <is>
           <t>agostino d.</t>
         </is>
       </c>
     </row>
     <row r="1954" ht="20" customHeight="1">
-      <c r="A1954" s="27" t="n">
+      <c r="A1954" s="26" t="n">
         <v>45170</v>
       </c>
     </row>
     <row r="1955" ht="20" customHeight="1">
-      <c r="A1955" s="4" t="inlineStr">
+      <c r="A1955" s="3" t="inlineStr">
         <is>
           <t>Abbiamo soggiornato in questo stupendo luogo subito dopo ferragosto, per una settimana. Acqua splendida, casa ottima con tutto quello che serve, location veramente stupenda. Il proprietario, Francesco, è persona gentilissima e molto disponibile. E i dintorni, le Madonie e Cefalù, veramente da visitare. Ottima scelta</t>
         </is>
       </c>
     </row>
     <row r="1956" ht="20" customHeight="1">
-      <c r="A1956" s="15" t="inlineStr">
+      <c r="A1956" s="14" t="inlineStr">
         <is>
           <t>read more</t>
         </is>
       </c>
     </row>
     <row r="1959" ht="20" customHeight="1">
-      <c r="A1959" s="4" t="inlineStr">
+      <c r="A1959" s="3" t="inlineStr">
         <is>
           <t>5 of 5 reviews</t>
         </is>
       </c>
     </row>
     <row r="1960" ht="20" customHeight="1">
-      <c r="A1960" s="15" t="n"/>
+      <c r="A1960" s="14" t="n"/>
     </row>
     <row r="1961" ht="20" customHeight="1">
-      <c r="A1961" s="15" t="n"/>
+      <c r="A1961" s="14" t="n"/>
     </row>
     <row r="1962" ht="31" customHeight="1">
-      <c r="A1962" s="14" t="inlineStr">
+      <c r="A1962" s="13" t="inlineStr">
         <is>
           <t>Enquire now</t>
         </is>
       </c>
     </row>
     <row r="1963" ht="23" customHeight="1">
-      <c r="A1963" s="29" t="inlineStr">
+      <c r="A1963" s="28" t="inlineStr">
         <is>
           <t>Aqua Turchina</t>
         </is>
       </c>
     </row>
     <row r="1964" ht="19" customHeight="1">
-      <c r="A1964" s="6" t="inlineStr">
+      <c r="A1964" s="5" t="inlineStr">
         <is>
           <t>5 Reviews</t>
         </is>
       </c>
     </row>
     <row r="1965" ht="34" customHeight="1">
-      <c r="A1965" s="8" t="inlineStr">
+      <c r="A1965" s="7" t="inlineStr">
         <is>
           <t>location_on Cefalù (Palermo)</t>
         </is>
       </c>
     </row>
     <row r="1966" ht="20" customHeight="1">
-      <c r="A1966" s="15" t="inlineStr">
+      <c r="A1966" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve">Name </t>
         </is>
       </c>
     </row>
     <row r="1967" ht="20" customHeight="1">
-      <c r="A1967" s="15" t="inlineStr">
+      <c r="A1967" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve">Surname </t>
         </is>
       </c>
     </row>
     <row r="1968" ht="20" customHeight="1">
-      <c r="A1968" s="15" t="inlineStr">
+      <c r="A1968" s="14" t="inlineStr">
         <is>
           <t>Nationality                              Afghanistan                             Albania                             Algeria                             American Samoa                             Andorra                             Angola                             Anguilla                             Antarctica                             Antigua and Barbuda                             Argentina                             Armenia                             Aruba                             Australia                             Austria                             Azerbaijan                             Bahamas                             Bahrain                             Bangladesh                             Barbados                             Belarus                             Belgium                             Belize                             Benin                             Bermuda                             Bhutan                             Bolivia                             Bosnia and Herzegovina                             Botswana                             Bouvet Island                             Brazil                             British Indian Ocean Territory                             Brunei                             Bulgaria                             Burkina Faso                             Burundi                             Cambodia                             Cameroon                             Canada                             Cape Verde                             Cayman Islands                             Central African Republic                             Chad                             Chile                             China                             Christmas Island                             Cocos (Keeling) Islands                             Colombia                             Comoros                             Congo                             Cook Islands                             Costa Rica                             Croatia                             Cuba                             Cyprus                             Czech Republic                             Denmark                             Djibouti                             Dominica                             Dominican Republic                             East Timor                             Ecuador                             Egypt                             El Salvador                             Equatorial Guinea                             Eritrea                             Estonia                             Ethiopia                             Falkland Islands                             Faroe Islands                             Fiji Islands                             Finland                             France                             French Guiana                             French Polynesia                             French Southern territories                             Gabon                             Gambia                             Georgia                             Germany                             Ghana                             Gibraltar                             Greece                             Greenland                             Grenada                             Guadeloupe                             Guam                             Guatemala                             Guernsey                             Guinea                             Guinea-Bissau                             Guyana                             Haiti                             Heard Island and McDonald Islands                             Holy See (Vatican City State)                             Honduras                             Hong Kong                             Hungary                             Iceland                             India                             Indonesia                             Iran                             Iraq                             Ireland                             Isle of Man                             Israel                             Italy                             Ivory Coast                             Jamaica                             Japan                             Jersey                             Jordan                             Kazakhstan                             Kenya                             Kiribati                             Kuwait                             Kyrgyzstan                             Laos                             Latvia                             Lebanon                             Lesotho                             Liberia                             Libyan Arab Jamahiriya                             Liechtenstein                             Lithuania                             Luxembourg                             Macao                             North Macedonia                             Madagascar                             Malawi                             Malaysia                             Maldives                             Mali                             Malta                             Marshall Islands                             Martinique                             Mauritania                             Mauritius                             Mayotte                             Mexico                             Micronesia, Federated States of                             Moldova                             Monaco                             Mongolia                             Montenegro                             Montserrat                             Morocco                             Mozambique                             Myanmar                             Namibia                             Nauru                             Nepal                             Netherlands                             Netherlands Antilles                             New Caledonia                             New Zealand                             Nicaragua                             Niger                             Nigeria                             Niue                             Norfolk Island                             North Korea                             Northern Ireland                             Northern Mariana Islands                             Norway                             Oman                             Pakistan                             Palau                             Palestine                             Panama                             Papua New Guinea                             Paraguay                             Peru                             Philippines                             Pitcairn                             Poland                             Portugal                             Puerto Rico                             Qatar                             Reunion                             Romania                             Russia                             Rwanda                             Saint Helena                             Saint Kitts and Nevis                             Saint Lucia                             Saint Pierre and Miquelon                             Saint Vincent and the Grenadines                             Samoa                             San Marino                             Sao Tome and Principe                             Saudi Arabia                             Senegal                             Serbia                             Seychelles                             Sierra Leone                             Singapore                             Slovakia                             Slovenia                             Solomon Islands                             Somalia                             South Africa                             South Georgia and the South Sandwich Islands                             South Korea                             South Sudan                             Spain                             Sri Lanka                             Sudan                             Suriname                             Svalbard and Jan Mayen                             Swaziland                             Sweden                             Switzerland                             Syria                             Tajikistan                             Tanzania                             Thailand                             The Democratic Republic of Congo                             Timor-Leste                             Togo                             Tokelau                             Tonga                             Trinidad and Tobago                             Tunisia                             Turkey                             Turkmenistan                             Turks and Caicos Islands                             Tuvalu                             Uganda                             Ukraine                             United Arab Emirates                             United Kingdom                             United States                             United States Minor Outlying Islands                             Uruguay                             Uzbekistan                             Vanuatu                             Venezuela                             Vietnam                             Virgin Islands, British                             Virgin Islands, U.S.                             Wallis and Futuna                             Western Sahara                             Yemen                             Zambia                             Zimbabwe                     Italy</t>
         </is>
       </c>
     </row>
     <row r="1969" ht="20" customHeight="1">
-      <c r="A1969" s="15" t="inlineStr">
+      <c r="A1969" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve">Phone </t>
         </is>
       </c>
     </row>
     <row r="1970" ht="20" customHeight="1">
-      <c r="A1970" s="15" t="inlineStr">
+      <c r="A1970" s="14" t="inlineStr">
         <is>
           <t>Italy +39</t>
         </is>
       </c>
     </row>
     <row r="1971" ht="20" customHeight="1">
-      <c r="A1971" s="15" t="n">
+      <c r="A1971" s="14" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="1972" ht="20" customHeight="1">
-      <c r="A1972" s="15" t="inlineStr">
+      <c r="A1972" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve">Email </t>
         </is>
       </c>
     </row>
     <row r="1973" ht="20" customHeight="1">
-      <c r="A1973" s="15" t="inlineStr">
+      <c r="A1973" s="14" t="inlineStr">
         <is>
           <t>Check-inCheck-out</t>
         </is>
       </c>
     </row>
     <row r="1974" ht="18" customHeight="1">
-      <c r="A1974" s="19" t="inlineStr">
+      <c r="A1974" s="18" t="inlineStr">
         <is>
           <t>pick a datepick a date</t>
         </is>
       </c>
     </row>
     <row r="1975" ht="20" customHeight="1">
-      <c r="A1975" s="15" t="inlineStr">
+      <c r="A1975" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve"> I don't have a date scheduled</t>
         </is>
       </c>
     </row>
     <row r="1976" ht="20" customHeight="1">
-      <c r="A1976" s="15" t="inlineStr">
+      <c r="A1976" s="14" t="inlineStr">
         <is>
           <t>Guests0 adult 0 child 0 infant 0 pet</t>
         </is>
       </c>
     </row>
     <row r="1977" ht="20" customHeight="1">
-      <c r="A1977" s="15" t="inlineStr">
+      <c r="A1977" s="14" t="inlineStr">
         <is>
           <t>Bedrooms0 bedroom</t>
         </is>
       </c>
     </row>
     <row r="1978" ht="20" customHeight="1">
-      <c r="A1978" s="15" t="inlineStr">
+      <c r="A1978" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve">Message </t>
         </is>
       </c>
     </row>
     <row r="1979" ht="20" customHeight="1">
-      <c r="A1979" s="15" t="inlineStr">
+      <c r="A1979" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve"> I've read and agree to the Privacy Policy and the Terms &amp; Conditions</t>
         </is>
       </c>
     </row>
     <row r="1980" ht="20" customHeight="1">
-      <c r="A1980" s="15" t="inlineStr">
+      <c r="A1980" s="14" t="inlineStr">
         <is>
           <t>Send request</t>
         </is>
       </c>
     </row>
     <row r="1981" ht="21" customHeight="1">
-      <c r="A1981" s="30" t="n"/>
+      <c r="A1981" s="29" t="n"/>
     </row>
     <row r="1982" ht="21" customHeight="1">
-      <c r="A1982" s="31" t="inlineStr">
+      <c r="A1982" s="30" t="inlineStr">
         <is>
           <t>Your wish for a villa escape</t>
         </is>
       </c>
     </row>
     <row r="1985" ht="25" customHeight="1">
-      <c r="A1985" s="32" t="inlineStr">
+      <c r="A1985" s="31" t="inlineStr">
         <is>
           <t>About us</t>
         </is>
@@ -8505,7 +8238,7 @@
       </c>
     </row>
     <row r="1990" ht="25" customHeight="1">
-      <c r="A1990" s="32" t="inlineStr">
+      <c r="A1990" s="31" t="inlineStr">
         <is>
           <t>Customers</t>
         </is>
@@ -8540,7 +8273,7 @@
       </c>
     </row>
     <row r="1995" ht="25" customHeight="1">
-      <c r="A1995" s="32" t="inlineStr">
+      <c r="A1995" s="31" t="inlineStr">
         <is>
           <t>Destinations</t>
         </is>
@@ -8582,7 +8315,7 @@
       </c>
     </row>
     <row r="2001" ht="25" customHeight="1">
-      <c r="A2001" s="32" t="inlineStr">
+      <c r="A2001" s="31" t="inlineStr">
         <is>
           <t>Owners</t>
         </is>
@@ -8617,45 +8350,45 @@
       </c>
     </row>
     <row r="2006" ht="21" customHeight="1">
-      <c r="A2006" s="31" t="inlineStr">
+      <c r="A2006" s="30" t="inlineStr">
         <is>
           <t>Support Sicily srl</t>
         </is>
       </c>
     </row>
     <row r="2007" ht="21" customHeight="1">
-      <c r="A2007" s="31" t="inlineStr">
+      <c r="A2007" s="30" t="inlineStr">
         <is>
           <t>VAT IT06182930823</t>
         </is>
       </c>
     </row>
     <row r="2008" ht="21" customHeight="1">
-      <c r="A2008" s="31" t="inlineStr">
+      <c r="A2008" s="30" t="inlineStr">
         <is>
           <t>Via Uditore, 11/H, 90145</t>
         </is>
       </c>
     </row>
     <row r="2009" ht="21" customHeight="1">
-      <c r="A2009" s="31" t="inlineStr">
+      <c r="A2009" s="30" t="inlineStr">
         <is>
           <t>Palermo, Italy</t>
         </is>
       </c>
     </row>
     <row r="2010" ht="21" customHeight="1">
-      <c r="A2010" s="30" t="n"/>
+      <c r="A2010" s="29" t="n"/>
     </row>
     <row r="2013" ht="19" customHeight="1">
-      <c r="A2013" s="33" t="inlineStr">
+      <c r="A2013" s="32" t="inlineStr">
         <is>
           <t>© 2025 Wish Sicily · Terms &amp; conditions · Privacy policy · Press room · Collections</t>
         </is>
       </c>
     </row>
     <row r="2014" ht="19" customHeight="1">
-      <c r="A2014" s="33" t="inlineStr">
+      <c r="A2014" s="32" t="inlineStr">
         <is>
           <t>€EUR</t>
         </is>

</xml_diff>

<commit_message>
feat(xlsx): check if xlsx is open and raise an error
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,68 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francorodrigo\Desktop\ClicketTest\Ingenarte_AutoClicker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8399E32B-290A-4523-96EC-651826DAB213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-61320" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B91C62B4-A470-42A1-8D07-A8DF16A7F13A}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-61320" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>www.yahoo.com.ar</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -79,26 +52,85 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -398,23 +430,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF3ED1D-7CB3-492B-B5AA-401E7689218C}">
-  <dimension ref="A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>www.yahoo.com.ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def process_step(tab_name, step_number, step_config):
+</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{5B3E4C1C-5BA0-4D7B-B351-DBCC1523A3C6}"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>